<commit_message>
Changes in property file for Supplier
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="749">
   <si>
     <t>Username</t>
   </si>
@@ -2394,10 +2394,34 @@
     <t>BEEPSEND-MT-SMPP-DIRECT [30040-6]</t>
   </si>
   <si>
-    <t>Error: Please enter all the mandatory fields.</t>
-  </si>
-  <si>
-    <t>Warning: This action will also submit the details for other instances and create an order. Do you want to Continue?</t>
+    <t>Please enter all mandatory input parameters.</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.NoSuchElementException: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@role='dialog']//button[span[text()='Yes' or text()='Ok']]"}
+  (Session info: chrome=60.0.3112.90)
+  (Driver info: chromedriver=2.29.461591 (62ebf098771772160f391d75e589dc567915b233),platform=Windows NT 10.0.10586 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 3.04 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.3.1', revision: '5234b325d5', time: '2017-03-10 09:10:29 +0000'
+System info: host: 'PAVILION', ip: '10.150.235.3', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_77'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.29.461591 (62ebf098771772160f391d75e589dc567915b233), userDataDir=C:\Users\Hp\AppData\Local\Temp\scoped_dir6744_18361}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=60.0.3112.90, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=}]
+Session ID: 8ffc709a643d83a47baeb28f3b3f324f
+*** Element info: {Using=xpath, value=//div[@role='dialog']//button[span[text()='Yes' or text()='Ok']]}</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.InvalidSelectorException: invalid selector: Unable to locate an element with the xpath expression ////button[contains(text(),'Ok')] because of the following error:
+SyntaxError: Failed to execute 'evaluate' on 'Document': The string '////button[contains(text(),'Ok')]' is not a valid XPath expression.
+  (Session info: chrome=60.0.3112.90)
+  (Driver info: chromedriver=2.29.461591 (62ebf098771772160f391d75e589dc567915b233),platform=Windows NT 10.0.10586 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 46 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/invalid_selector_exception.html
+Build info: version: '3.3.1', revision: '5234b325d5', time: '2017-03-10 09:10:29 +0000'
+System info: host: 'PAVILION', ip: '10.150.235.3', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_77'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.29.461591 (62ebf098771772160f391d75e589dc567915b233), userDataDir=C:\Users\Hp\AppData\Local\Temp\scoped_dir7812_5937}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=60.0.3112.90, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, unexpectedAlertBehaviour=}]
+Session ID: 6aab1408b88c4471aaeb464837c60eb5
+*** Element info: {Using=xpath, value=////button[contains(text(),'Ok')]}</t>
   </si>
 </sst>
 </file>
@@ -8652,8 +8676,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BY16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0" zoomScale="95" zoomScaleNormal="95">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9159,7 +9183,7 @@
         <v>107</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="26.25" r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -9184,11 +9208,11 @@
       <c r="H6" t="s">
         <v>122</v>
       </c>
-      <c r="I6" t="s">
-        <v>462</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>29</v>
+      <c r="I6" s="25" t="s">
+        <v>746</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>744</v>
       </c>
       <c r="K6" s="5"/>
       <c r="P6" s="5" t="s">

</xml_diff>

<commit_message>
Validation of options in fixed dropdown
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="5" tabRatio="855" windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="22" firstSheet="20" tabRatio="855" windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Provisioning_Screen" r:id="rId1" sheetId="24"/>
@@ -29,17 +29,18 @@
     <sheet name="Checking_Roles_Access" r:id="rId20" sheetId="13"/>
     <sheet name="Customer_Coverage_Screen" r:id="rId21" sheetId="7"/>
     <sheet name="ValidatingFields_Roles" r:id="rId22" sheetId="14"/>
-    <sheet name="ScreenAccessBasedOnRoles" r:id="rId23" sheetId="15"/>
-    <sheet name="Custom_Error_Screen" r:id="rId24" sheetId="28"/>
-    <sheet name="XML_Comparison" r:id="rId25" sheetId="29"/>
-    <sheet name="RetryScheme" r:id="rId26" sheetId="30"/>
+    <sheet name="ValidatingOptions_FixedDropdown" r:id="rId23" sheetId="31"/>
+    <sheet name="ScreenAccessBasedOnRoles" r:id="rId24" sheetId="15"/>
+    <sheet name="Custom_Error_Screen" r:id="rId25" sheetId="28"/>
+    <sheet name="XML_Comparison" r:id="rId26" sheetId="29"/>
+    <sheet name="RetryScheme" r:id="rId27" sheetId="30"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3385" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3605" uniqueCount="1033">
   <si>
     <t>Username</t>
   </si>
@@ -2876,10 +2877,365 @@
 - Check Ediatbale and Non-editable funtionality based on coverage checkbox</t>
   </si>
   <si>
-    <t>Error: Please provide at least one Route feature.</t>
-  </si>
-  <si>
-    <t>Warning: This action will upload the Selected CSV. Do you want to Continue ?</t>
+    <t>PT_InstanceLst_Val</t>
+  </si>
+  <si>
+    <t>ALL;MTTSMSHUB1;MTTSMSHUB2;MTTSMSHUB9;TTTSMSHUB1;TTTSMSHUB2;TTTSMSHUB9</t>
+  </si>
+  <si>
+    <t>ALL;ABKHAZIA;AFGHANISTAN;ALBANIA;ALGERIA;AMERICAN SAMOA;ANDORRA;ANGOLA;ANGUILLA;ANTIGUA &amp; BARB;ARGENTINA;ARMENIA;ARUBA;AUSTRALIA;AUSTRIA;AZERBAIJAN;BAHAMAS;BAHRAIN;BANGLADESH;BARBADOS;BELARUS;BELGIUM;BELIZE;BENIN;BERMUDA;BHUTAN;BOLIVIA;BOSNIA-HERZEG.;BOTSWANA;BR VIRGIN ISL;BRAZIL;BRUNEI;BULGARIA;BURKINA FASO;BURUNDI;CAMBODIA;CAMEROON;CANADA;CAPE VERDE;CAYMAN ISLANDS;CENTRAL AFRICA;CHAD;CHILE;CHINA;COLOMBIA;COMOROS;CONGO;COOK ISLANDS;COSTA RICA;COTE D IVOIRE;CROATIA;CUBA;CYPRUS;CZECH (REP);DEM REP CONGO;DENMARK;DJIBOUTI;DOMINICA;DOMINICAN REP;EAST TIMOR;ECUADOR;EGYPT;EL SALVADOR;EQUA GUINEA;ESTONIA;ETHIOPIA;FALKLAND ISL.;FAROE ISLANDS;FIJI;FINLAND;FR. POLYNESIA;FRANCE;FRENCH GUIANA;GABON;GAMBIA;GEORGIA;GERMANY;GHANA;GIBRALTAR;GREECE;GREENLAND;GRENADA;GUADELOUPE;GUAM;GUATEMALA;GUINEA;GUINEA-BISSAU;GUYANA;HAITI;HONDURAS;HONG KONG;HUNGARY;ICELAND;INDIA;INDONESIA;IRAN;IRAQ;IRELAND;ISRAEL;ITALY;JAMAICA;JAPAN;JORDAN;KAZAKHSTAN;KENYA;KUWAIT;KYRGYZSTAN;LAOS;LATVIA;LEBANON;LESOTHO;LIBERIA;LIBYA;LIECHTENSTEIN;LITHUANIA;LUXEMBOURG;MACAU;MACEDONIA;MADAGASCAR;MALAWI;MALAYSIA;MALDIVES;MALI;MALTA;MAURITANIA;MAURITIUS;MEXICO;MICRONESIA;MOLDOVA;MONACO;MONGOLIA;MONTENEGRO;MONTSERRAT;MOROCCO;MOZAMBIQUE;MYANMAR;NAMIBIA;NEPAL;NETH ANTILLES;NETHERLANDS;NEW CALEDONIA;NEW ZEALAND;NICARAGUA;NIGER;NIGERIA;NORTH MARIANAS;NORWAY;OMAN;PAKISTAN;PALAU;PALESTINE;PANAMA;PAPUA N.G.;PARAGUAY;PERU;PHILIPPINES;POLAND;PORTUGAL;PUERTO RICO;QATAR;REUNION;ROMANIA;RUSSIA;RWANDA;SAINT LUCIA;SAMOA;SAN MARINO;SAO TOME/PRINC.;SAUDI ARABIA;SENEGAL;SERBIA;SEYCHELLES;SIERRA LEONE;SINGAPORE;SLOVAKIA;SLOVENIA;SOLOMON ISLANDS;SOMALIA;SOUTH AFRICA;SOUTH KOREA;SOUTH SUDAN;SPAIN;SRI LANKA;ST KITTS/NEVIS;ST VINCENT &amp; GR;ST-PIERRE-MIQ.;SUDAN;SURINAME;SWAZILAND;SWEDEN;SWITZERLAND;SYRIA;TAIWAN;TAJIKISTAN;TANZANIA;THAILAND;TOGO;TONGA;TRINIDAD-TOBAGO;TUNISIA;TURKEY;TURKMENISTAN;TURKS &amp; CAICOS;UGANDA;UK;UKRAINE;UNIT. ARAB EMIR;UNITED STATES;URUGUAY;UZBEKISTAN;VANUATU;VENEZUELA;VIETNAM;YEMEN (ARAB);ZAMBIA;ZIMBABWE;</t>
+  </si>
+  <si>
+    <t>ALL;42 TELECOM;A-MOBILE;ADVANTAGE CELLULAR SYSTEMS;AERO MOBILE;AFGHAN TELECOM;AFGHAN WIRELESS;AFRICEL GAMBIA;AFRICELL;AFRICELL DRC;AFRICELL LINTEL SIERRA LEONE;AGILE TELECOM;AGILE TELECOM POLAND;AIN AWN GLOBAL COMMUNICATIONS;AIR TELECOM;AIRCEL ANDHRA PRADESH;AIRCEL ASSAM;AIRCEL BIHAR AND JHARKHAND;AIRCEL CELLULAR SMS AGGREGATOR;AIRCEL CHENNAI;AIRCEL DELHI;AIRCEL GUJARAT;AIRCEL HARYANA;AIRCEL HIMACHAL PRADESH;AIRCEL JAMMU AND KASHMIR;AIRCEL KARNATAKA;AIRCEL KERALA;AIRCEL KOLKATA;AIRCEL MADHYA PRADESH;AIRCEL MAHARASHTRA;AIRCEL MUMBAI;AIRCEL NORTH EAST;AIRCEL ORISSA;AIRCEL PUNJAB;AIRCEL RAJASTHAN;AIRCEL TAMILNADU;AIRCEL UTTAR PRADESH EAST;AIRCEL UTTAR PRADESH WEST;AIRCEL WEST BENGAL;AIRTEL ASSAM;AIRTEL BIHAR;AIRTEL JAMMU AND KASHMIR;AIRTEL JERSEY;AIRTEL NETWORKS ZAMBIA;AIRTEL NORTH EAST;AIRTEL ORISSA;AIRTEL RWANDA;AIRTEL UP EAST;AIRTEL WEST BENGAL;AIS 2G;ALANDS MOBILTELEFON;ALASKA DIGITEL;ALBANIAN MOBILE COMMUNICATIONS;ALFA TELECOM CJSC MEGACOM;ALGAR TELECOM;ALGERIE TELECOM MOBILE;ALJAWAL SAUDI TELECOM COMPANY;ALLCOMMUNICATIONS LIECHTENSTEIN;ALLTEL;ALTEL KAZAKHSTAN;AMD TELECOM GREECE;AMD TELECOM POLAND;AMERICA MOVIL PERU;ANGOLA MOVICEL;ANTEL;APUA PCS;AREEBA AFGHANISTAN;AREEBA GUINEA;ARMENTEL;ASIA CELL TELECOMMUNICATIONS COMPANY;ASIA PACIFIC TELECOM;ASPENTA;ASTAC;ASTRIUM;AT&amp;T COMERCIALIZACION MOVIL;AT&amp;T COMUNICACIONES DIGITALES MEXICO;AT&amp;T EDGE WIRELESS;AT&amp;T WIRELESS;ATLANTIQUE CELLULAIRE;ATLANTIQUE CELLULAR;ATLANTIQUE TELECOM MOOV;AVANTEL;AXISPT NATRINDO TELEPON SELULER;AZERCELL;AZERFON;AZULES Y PLATAS TELEFONICA;B-MOBILE BHUTAN;B-MOBILE BRUNEI;BAKCELL;BANGLALINK SHEBA BANGLADESH;BARABLU SPAIN;BASE;BASHAIR TELECOM;BATELCO BAHRAIN TELECOMMUNICATIONS;BAYKALWESTCOM RUSKH;BEELINE LAO;BELIZE TELEMEDIA;BELL MOBILITY;BELLBENIN COMMUNICATIONS;BEMOBILE;BERMUDA DIGITAL COMMUNICATIONS;BEST;BH TELECOM;BHARAT SANCHAR NIGAM CELONE;BHARTI AIRTEL LANKA;BHARTI AIRTEL SMS AGGREGATOR;BHARTI CELLULAR ANDHRA PRADESH;BHARTI CELLULAR CHENNAI;BHARTI CELLULAR DELHI;BHARTI CELLULAR GUJARAT;BHARTI CELLULAR HARYANA;BHARTI CELLULAR HIMACHAL PRADESH;BHARTI CELLULAR KARNATAKA;BHARTI CELLULAR KERALA;BHARTI CELLULAR KOLKATA;BHARTI CELLULAR MADHYA PRADESH;BHARTI CELLULAR MAHARASHTRA;BHARTI CELLULAR MUMBAI;BHARTI CELLULAR PUNJAB;BHARTI CELLULAR TAMILNADU;BHARTI CELLULAR UPWEST;BHARTI HEXCOM;BITE GSM;BLUE SKY COMMUNICATIONS;BOTSWANA TELECOMMUNICATIONS CORPORATION;BOUYGUES TELECOM;BRAGG COMMUNICATIONS;BROADPOINT USA;BSNL ANDHRA PRADESH;BSNL ASSAM;BSNL BIHAR;BSNL CHENNAI;BSNL GUJARAT;BSNL HARYANA;BSNL HIMACHAL PRADESH;BSNL JAMMU AND KASHMIR;BSNL KARNATAKA;BSNL KERALA;BSNL KOLKATA;BSNL MADHYA PRADESH;BSNL MAHARASHTRA;BSNL NORTH EAST;BSNL ORISSA;BSNL PUNJAB;BSNL RAJASTAN;BSNL SMS AGGREGATOR;BSNL TAMIL NADU;BSNL UTTAR PRADESH EAST;BSNL UTTAR PRADESH WEST;BT ITALIA;BUG TUSSEL WIRELESS;CABLE&amp;WIRELESS ANGUILLA;CABLE&amp;WIRELESS ANTIGUA AND BARBUDA;CABLE&amp;WIRELESS BARBADOS;CABLE&amp;WIRELESS BRITISH VIRGIN ISLANDS;CABLE&amp;WIRELESS CAYMAN;CABLE&amp;WIRELESS DOMINICA;CABLE&amp;WIRELESS GRENADA;CABLE&amp;WIRELESS JAMAICA;CABLE&amp;WIRELESS MONTSERRAT;CABLE&amp;WIRELESS PANAMA;CABLE&amp;WIRELESS SEYCHELLES;CABLE&amp;WIRELESS ST-KITTS AND NEVIS;CABLE&amp;WIRELESS ST-LUCIA;CABLE&amp;WIRELESS ST-VINCENT;CABLE&amp;WIRELESS TURKS AND CAICOS;CABLE&amp;WIRELESS UNITED KINGDOM;CABO VERDE TELECOM CV MOVEL;CADCOMMS;CAMGSM COMPANY METFONE;CARDBOARDFISH;CARPHONE WAREHOUSE IRELAND MOBILE;CCT BOATPHONE;CELCOM AXIATA BERHAD;CELL C;CELLCOM ISRAEL;CELLCOM TELECOMMUNICATIONS;CELLCOM TELECOMMUNICATIONS1;CELLONE;CELLPLUS MOBILE COMMUNICATIONS;CELLULAR ONE 310320;CELLULAR ONE 310570;CELLULAR ONE OF EAST CENTRAL ILLINOIS;CELLZ;CELTEL BRAZZAVILLE;CELTEL BURKINA FASO;CELTEL CHAD;CELTEL DRC;CELTEL GABON;CELTEL KENYA;CELTEL MALAWI;CELTEL NIGER;CELTEL SIERRA LEONE;CELTEL TANZANIA;CELTEL UGANDA;CENTERTEL IDEA;CHARITON VALLEY WIRELESS;CHINA MOBILE;CHINA SPACECOM MOBILE TELECOMMUNICATIONS;CHINA TELECOM;CHINA UNICOM HONG KONG;CHINA UNICOM MOBILE;CHINE TELECOM DRC;CHINGUITEL;CHOICE PHONE;CHOICE WIRELESS;CHUNGHWA TELECOM CO MOBILE;CINCINNATI BELL TELEPHONE;CITIC TELECOM;CLARO BRAZIL;CLARO COSTA RICA;CLARO DOMINICANA;CLARO HONDURAS;CLARO JAMAICA;CLARO NICARAGUA;CLARO PANAMA;CLARO PARAGUAY;CLARO PUERTO RICO;CLARO SERCOM;CLARO SMARTCOM;CLOUD9;CLX NETWORKS;COLOMBIA MOVIL;COM4 NORWAY;COMCEL VOILA;COMFONE ATHEER TELECOM;COMIUM;COMIUM GAMBIA;COMIUM SIERRA LEONE;COMMUNICATION FOR DEVICES IN SWEDEN;COMNET WIRELESS;COMORES TELECOM;COMUNICACION CELULAR;COMUNICACIONES CELULARES COMCEL;CONSORCIO ECUATORIANO DE TELECOMUNICACIO;COOL TEL;CORPORACION DIGITEL;CORR WIRELESS;COSCOM;COSMO BULGARIA MOBILE GLOBUL;COSMOFON MACEDONIA;COSMOTE;COSMOTE COSMOROM;CSTMOVEL;CTC TELCOM DBA MOSAIC TELECOM;CTE TELECOM PERSONAL;CTI AMERICA MOVIL;CTI URUGUAY AM WIRELESS;CTM COMPANHIA TELECOM MACAU;CTS GIBRALTAR;CUBIC TELECOM;CURE;DACOM CORPORATION;DATA&amp;AUDIO-VISUAL ENTERPRISES WIRELESS;DAUPHIN TELECOM;DHIRAAGU DHIMOBILE MALDIVES;DIALOG TELEKOM;DIALOGUE;DIGI TELECOMMUNICATIONS;DIGICEL ANGUILLA;DIGICEL ANTIGUA AND BARBUDA;DIGICEL ARUBA;DIGICEL BARBADOS;DIGICEL BERMUDA;DIGICEL BRITISH VIRGIN ISLANDS;DIGICEL CAYMAN;DIGICEL CURACAO;DIGICEL DOMINICA;DIGICEL EL SALVADOR;DIGICEL FIJI;DIGICEL FRENCH WEST INDIES;DIGICEL GRENADA;DIGICEL GUYANA;DIGICEL HAITI;DIGICEL JAMAICA;DIGICEL JAMAICA3;DIGICEL LOTCS;DIGICEL PANAMA;DIGICEL PAPUA NEW GUINEA;DIGICEL SAMOA;DIGICEL ST-KITTS AND NEVIS;DIGICEL ST-LUCIA;DIGICEL ST-VINCENT;DIGICEL SURINAME;DIGICEL TONGA;DIGICEL TRINIDAD;DIGICEL TURKS AND CAICOS;DIGICEL VANUATU;DIGIMOBIL;DIGITAL NETWORK ACCESS COMMUNICATIONS;DIGITAL TELECOMMUNICATIONS PHILIPPINES;DJIBOUTI TELECOM;DOBSON COMMUNICATIONS CORPORATION;DONTELECOM ROSTOV TELECOM;DST COMMUNICATION DST1;DST COMMUNICATION DST2;DTAC TOTAL ACCESS COMMUNICATIONS;DTN DTAC NETWORK COMPANY;DU UNITED ARAB EMIRATES;E-LUX MOBILE;E-PLUS;EAGLE MOBILE;EAZITELECOM GIBRALTAR;ECONET EZI-CEL;ECONET WIRELESS;ECONET WIRELESS BURUNDI;EKATERINBURG-2000;ELISA ESTONIA;ELISA FINLAND;ELMADAR TELECOM COMPANY;ELSACOM;EMERY TELECOM WIRELESS USA;EMNIFY;EMOBILE;EMTEL;ENTEL MOVIL;ENTEL PCS;EQUATEUR TELECOM CONGO AZUR CANGO;ERONET;ESSAR TELECOM;ESTONIAN MOBILE TELEPHONE;ETECSA CCOM CUBACEL;ETHIOPIAN TELECOMMUNICATIONS CORPORATION;ETISALAT AFGHANISTAN;ETISALAT MISR;ETISALAT MOBILE NIGERIA;ETISALAT MOBILE UAE;ETK YENISEYTELECOM;ETL MOBILE;EUTEL;EXCELCOM;EXECULINK;EXPRESSO;FAR EASTONE TELECOMMUNICATIONS;FAROESE TELECOM;FINNET NETWORKS;FIRST CELLULAR OF SOUTHERN ILLINOIS;FISHTEXT UNITED KINGDOM;FIXED&amp;MOBILE;FONYOU SPAIN;FREE MOBILE FRANCE;FSM TELECOMMUNICATIONS CORPORATION;FSM TELECOMMUNICATIONS TUVALU;G MOBILE GEORGIA;G-MOBILE CORPORATION;GAMCEL;GAMMA TELECOM;GEMTEL;GENERAL COMMUNICATIONS USA;GEOCELL;GETESA;GIBTEL;GLO MOBILE GHANA;GLOBACOM GLO MOBILE;GLOBAL MESSAGE SERVICES UKRAINE;GLOBAL NETWORKS1;GLOBAL TELECOM;GLOBALIVE WIRELESS MANAGEMENT;GLOBALSTAR BRAZIL1;GLOBALSTAR EUROPE;GLOBALSTAR VODAFONE USA ANSI;GLOBALSTAR VODAFONE USA ITU;GLOBALTEL;GLOBE TELECOM;GLOBECOMM NETWORK;GLOBETOUCH;GLOMOBILE;GO MOBILE MOBLSLE COMMUNICATIONS;GOLAN TELECOM;GOLDEN TELECOM;GOLIS TELECOMMUNICATIONS COMPANY;GOTANET;GRAMEENPHONE;GREEN COM;GTEL MOBILE;GUYANA TELEPHONE TELEGRAPH;H3G ITALY;HAFATEL;HALYS;HAY SYSTEMS UNITED KINGDOM;HI3G ACCESS;HI3G DENMARK;HIGHLAND;HOLA PARAGUAY;HONG KONG CSL;HORMUUD TELECOM SOMALIA;HOT MOBILE;HUTCHISON SRILANKA;HUTCHISON TELECOM;HUTCHISON TELEPHONE MACAU;HUTCHISON3G AUSTRALIA;HUTCHISON3G AUSTRIA;HUTCHISON3G HONG KONG;HUTCHISON3G IRELAND;HUTCHISON3G UNITED KINGDOM;ICE CELLULAR COSTA RICA 71201;ICE WIRELESS;IDC MOLDOVA;IDEA CELLULAR ANDHRA PRADESH;IDEA CELLULAR ASSAM;IDEA CELLULAR BIHAR AND JHARKHAND;IDEA CELLULAR DELHI;IDEA CELLULAR GUJARAT;IDEA CELLULAR HARYANA;IDEA CELLULAR HIMACHAL PRADESH;IDEA CELLULAR JAMMU AND KASHMIR;IDEA CELLULAR KARNATAKA;IDEA CELLULAR KERALA;IDEA CELLULAR KOLKATA;IDEA CELLULAR MADHYA PRADESH;IDEA CELLULAR MAHARASHTRA;IDEA CELLULAR MUMBAI;IDEA CELLULAR NORTH EAST;IDEA CELLULAR ORISSA;IDEA CELLULAR PUNJAB;IDEA CELLULAR RAJASTHAN;IDEA CELLULAR SMS AGGREGATOR;IDEA CELLULAR TAMIL NADU AND CHENNAI;IDEA CELLULAR UTTAR PRADESH EAST;IDEA CELLULAR UTTAR PRADESH WEST;IDEA CELLULAR WEST BENGAL;IMC ISLAND;IMETRIK GLOBAL;IMEZ;IN&amp;PHONE;INDIGO WIRELESS;INMARSAT;INTERCEL GUINEE;IOWA WIRELESS SERVICES;ISLANDCOM TELECOMMUNICATIONS;ISMART MOBILE;IT&amp;E WIRELESS;ITISSALAT AL MAGHRIB;JASPER WIRELESS;JAZZTEL;JERSEY TELECOMMUNICATIONS;JOSA BABILON MOBILE;K-TELECOM;KALL;KAPLAN TELEPHONE COMPANY;KAR TEL MOBILE;KARABAKH TELECOM;KCELL;KDDI CORPORATION JAPAN;KEEWAYTINOOK OKIMAKANAK;KEYSTONE WIRELESS;KG TELECOMMUNICATIONS;KINETO WIRELESS;KOREK TELECOM;KPN;KPN SPAIN;KT FREETEL;KTC KUWAIT;KYIVSTAR GSM;LACELL;LAO TELECOMMUNICATIONS;LATELZ CAMBODIA;LATVIAN MOBILE TELEPHONE;LETAI;LG UPLUS;LGI MOBILE UPC;LGI MOBILE UPC AUSTRIA;LGI MOBILE UPC IRELAND;LIBERCELL ATLANTIC WIRELESS;LIBERCOM;LIBERTIS GABON;LIBERTIS TELECOM;LIBYANA MOBILE;LIFECELL;LIFFEY TELECOM;LIMITLESS MOBILE;LOCAL EXCHANGE GLOBAL OPERATION SERVICES;LONESTARCELL;LONG LINES WIRELESS;LOOP MOBILE INDIA;LOOP MOBILE SMS AGGREGATOR;LOTENY TELECOM;LYCA MOBILE;LYCAMOBILE AUSTRALIA;LYCAMOBILE BELGIUM;LYCAMOBILE FRANCE;LYCAMOBILE GERMANY;LYCAMOBILE NETHERLANDS;LYCAMOBILE SPAIN;LYNX MOBILITY;M-TEL NIGERIA;MACH END2END MOBILE MIGWAY;MADACOM CELTEL;MAGTICOM;MAHANAGAR TELEPHONE MAURITIUS;MAHANAGAR TELEPHONE NIGAM DELHI;MAHANAGAR TELEPHONE NIGAM MUMBAI;MAINE PCS;MALITEL;MANX TELECOM;MARATHON TELECOM;MARITIME COMMUNICATIONS PARTNER;MASCOM WIRELESS;MATTEL GSM;MAURITEL MOBILES;MAXIS INTERNATIONAL;MCI IRAN;MEDI TELECOM;MEGAFON;MELITA MOBILE;MERCURY INTERNATIONAL CARRIER SERVICES;METEOR MOBILE COMMUNICATIONS;METFONE VIETEL CAMBODIA;METRO PCS USA;MIC1 LEBANON;MILLICOM CHAD;MILLICOM GHANA;MITTO SWITZERLAND;MOBICOM;MOBILAND ANDORRA;MOBILCOM MULTIMEDIA GERMANY;MOBILE TELECOMMUNICATIONS NAMIBIA;MOBILE TELEPHONE NETWORK;MOBILE TELEPHONE NETWORK MTNIRANCELL;MOBILEONE;MOBILINK;MOBILKOM;MOBILKOM LIECHTENSTEIN;MOBILTEL;MOBILTEL MIC TANZANIA;MOBILY ETIHAD ETILSAT;MOBIMAK;MOBINIL;MOBIQUI THINGS;MOBISTAR;MOBITEL;MOBITEL SRI LANKA;MOBIWEB DENMARK;MOBIWEB GREECE;MOBIWEB LUXEMBOURG;MOBIWEB POLAND;MOBIWEB SWEDEN;MOCAMBIQUE CELULAR MOZAMBIQUE;MOLDCELL MOLDOVA;MOLDTELECOM;MONACO TELECOM;MONACO TELECOM M2M;MONACO VALA900;MOOV TELECEL BENIN;MOOV TELECEL TOGO;MOVILNET;MOVITEL MOZAMBIQUE;MTC LEBANON;MTEL AUSTRIJA;MTEL PODGORICA;MTN AREEBA SPACETEL SYRIA;MTN CAMEROON;MTN NIGERIA;MTN RWANDACELL;MTN SOUTH SUDAN;MTN UGANDA;MTN ZAMBIA;MTNL SMS AGGREGATOR;MTS ALLSTREAM;MTS BELARUS;MTS DELHI;MTS GUJARAT;MTS KARNATAKA;MTS KERALA;MTS KOLKATA;MTS MOBILE TELESYSTEMS;MTS TAMIL NADU;MTS TURKMENISTAN;MTS UP WEST;MTS WEST BENGAL;MTX CONNECT;MULTIREGIONAL TRANSIT TELECOM;MUNDIO MOBILE AUSTRIA;MUNDIO MOBILE BELGIUM;MUNDIO MOBILE DENMARK;MUNDIO MOBILE FRANCE;MUNDIO MOBILE GB;MUNDIO MOBILE NETHERLANDS;MUNDIO MOBILE PORTUGAL;MUNDIO SWEDEN;MYANMA POSTS AND TELECOMMUNICATIONS;NATCOM HAITI;NATIONAL LINK;NATIONLINK TELECOM;NAVITAS TELECOM;NAWRAS;NCC NIZHEGORODSKAYA CELLULAR;NE COLORADO CELLULAR VIAERO USA;NEO;NEPAL TELECOMMUNICATIONS CORPORATION;NETCOM;NETONE;NEW DIMENSION WIRELESS USA;NEW TELEPHONE COMPANY;NEWCORE WIRELESS;NEXTEL PERU 3G;NEXTEL TELECOMUNICACOES 3G;NII HOLDINGS ARGENTINA;NII HOLDINGS BRAZIL;NII HOLDINGS CHILE;NII HOLDINGS MEXICO;NII HOLDINGS PERU;NORFOLK TELECOM;NORTHEAST NETWORKS WIRELESS;NOVA;NOVA OI MOVEL;NOVERCA;NPI WIRELESS;NRJ MOBILE;NTT COMMUNICATIONS;NUCLEO;NUEVATEL PCS DE BOLIVIA;NUMEREX;NURTELECOM;O2 CZECH REPUBLIC;O2 GERMANY;O2 IRELAND;O2 NETHERLANDS;O2 UNITED KINGDOM;OASIS;OI MOVEL;OMANTEL OMAN MOBILE;OMEA TELECOM;OMNITEL LITHUANIA;ONAIR SWITZERLAND;ONATEL MOBILE;ONE TOUCH GHANA TELECOMS;ONIWAY INFOCOMUNICACOES;ONMARINE SWITZERLAND;ONO SPAIN;OOREDOO MALDIVES;OOREDOO MYANMAR;OOREDOO TUNISIE;OPT NEW CALEDONIA;OPTIMUS;ORANGE;ORANGE BISSAU;ORANGE BOTSWANA VISTA;ORANGE CAMEROUN;ORANGE CARAIBE;ORANGE CENTRAFRIQUE;ORANGE COTE D IVOIRE;ORANGE DOMINICANA;ORANGE FRANCE;ORANGE GUINEA CONAKRY;ORANGE LUXEMBOURG;ORANGE M2M FRANCE;ORANGE MADAGASCAR;ORANGE MOBILECOM;ORANGE NIGER;ORANGE ONE;ORANGE PCS UNITED KINGDOM;ORANGE RETEVISION MOVIL AMENA;ORANGE REUNION;ORANGE ROMANIA;ORANGE SENEGAL;ORANGE SLOVENSKO;ORANGE TUNISIA;ORANGE UGANDA;ORANGE VOXTEL;ORASCOM DJEZZY ALGERIA;ORICEL COTE D IVOIRE;OUTREMER TELECOM;OUTREMER TELECOM FRENCH GUYANA;P&amp;T LUXEMBOURG;P4 POLAND;PACIFIC MOBILE;PACIFIC MOBILE COMMUNICATION B MOBILE;PAKTEL;PALAU MOBILE CORPORATION;PALAU MOBILE CORPORATION 3G;PALTEL;PANNON;PARIO SOLUTIONS;PARTNER ORANGE;PASIFIK SATELIT NUSANTARA;PCCW HONG KONG TELECOMMUNICATIONS;PELEPHONE COMMUNIATIONS;PEOPLES TELEPHONE;PINE TELEPHONE;PLATEAU TEL USA;PLUS COMMUNICATION;PNCC WIRELESS;POLKOMTEL;PRIMETEL;PRIMTELEFON;PRIVATE MOBILITY NETHERLANDS;PROMONTE GSM;PROSODIE;PROXIMUS;PT HUTCHISON CP TELECOMMUNICATIONS;PT INDOSAT;PTI PACIFICA;PULSE MOBILE GUAM;Q-TEL QATARNET;QCELL;QUAM GERMANY;RADIOMOVIL TELCEL;RCS&amp;RDS;REAL FUTURE;REAL MOVE;RELIANCE ASSAM;RELIANCE COMMUNICATIONS ANDHRA PRADESH;RELIANCE COMMUNICATIONS DELHI;RELIANCE COMMUNICATIONS GUJARAT;RELIANCE COMMUNICATIONS HARYANA;RELIANCE COMMUNICATIONS JAMMU;RELIANCE COMMUNICATIONS KARNATAKA;RELIANCE COMMUNICATIONS KERALA;RELIANCE COMMUNICATIONS MAHARASHTRA;RELIANCE COMMUNICATIONS MUMBAI;RELIANCE COMMUNICATIONS PUNJAB;RELIANCE COMMUNICATIONS RAJASTHAN;RELIANCE COMMUNICATIONS SMS AGGREGATOR;RELIANCE COMMUNICATIONS TAMIL NADU;RELIANCE COMMUNICATIONS UP EAST;RELIANCE COMMUNICATIONS UP WEST;RELIANCE HIMACHAL PRADESH;RELIANCE INFOCOMM;RELIANCE JIO ANDHRA PRADESH;RELIANCE JIO ASSAM;RELIANCE JIO BIHAR;RELIANCE JIO DELHI;RELIANCE JIO GUJARAT;RELIANCE JIO HARYANA;RELIANCE JIO HIMACHAL PRADESH;RELIANCE JIO J&amp;K;RELIANCE JIO KARNATAKA;RELIANCE JIO KERALA;RELIANCE JIO KOLKATA;RELIANCE JIO MADHYA PRADESH;RELIANCE JIO MAHARASHTRA;RELIANCE JIO MUMBAI;RELIANCE JIO NORTH EAST;RELIANCE JIO ORISSA;RELIANCE JIO PUNJAB;RELIANCE JIO RAJASTHAN;RELIANCE JIO SMS AGGREGATOR;RELIANCE JIO TAMIL NADU;RELIANCE JIO UP EAST;RELIANCE JIO UP WEST;RELIANCE JIO WEST BENGAL;RELIANCE NORTH EAST;RELIANCE ORISSA;RESILIENT NETWORKS;RIGHTEL COMMUNICATION SERVICES;ROAMWARE NETHERLANDS;ROBI AXIATA;ROGERS FIDO;ROGERS WIRELESS;ROUTOMESSAGING UNITED KINGDOM;RS TELECOMMUNICATIONS;RT MOBILE;RURAL CELLULAR COMMUNICATIONS;SABAPHONE;SAFARICOM;SAGEBRUSH CELLULAR;SAHELCOM;SALT LIECHTENSTEIN;SALT SWITZERLAND;SAMOA TEL;SAN MARINO TELECOM;SAP MOBILE SERVICES USA2;SAP MOBILE SERVICES VERIZON;SASKTEL;SAUDI GLOBALSTAR;SCANCOM;SCANCOM AREEBA;SENTELTIGO SENEGAL;SERCOM;SETAR;SFR;SI MOBIL;SIBCHALLENCE;SILKNET;SIMINN ICELAND TELECOM;SIMSIM;SINGTEL MOBILE;SINGTEL OPTUS;SISTEMA SHYAM TELESERVICE SMS AGGREGATOR;SISTEMA SHYAM TELESERVICES;SK TELECOM;SKY MOBILE BITEL;SKYTEL;SMART COMMUNICATIONS;SMART SIERRA LEONE;SMART TANZANIA;SMARTCOM;SMARTFREN;SMARTONE;SMARTONE COMMUNICACOES MOVEIS;SMARTS SAMARA;SMARTS SARANSK;SMARTS UFA;SMARTS ULIANOVSK;SMARTS YAROSLAVL;SMARTS YOSHKAR-OLA;SMSRELAY;SOFT BANK MOBILE;SOLOMON TELEKOM SOLOMON ISLANDS;SOMAFONE;SOMTEL;SONOFON;SOTELGUI GUINEA;SOUTH CAROLINA PHONE;SOUTH EAST ASIA TELECOM;SOUTHERN LINC;SPACETEL;SPACETEL GUINEA BISSAU;SPACETEL YEMEN;SPEEDNET COMMUNICATIONS;SPICE NEPAL PRIVATE;SPM TELECOM;SPRINT;SPRINT NEXTEL COMMUNICATIONS;SRR;STAR TELECOM;STARHUB;STARHUB M2M;STC BAHRAIN;STOUR MARINE;SUDATEL;SUNRISE TDC SWITZERLAND;SURE GUERNSEY;SURE SOUTH ATLANTIC;SURE TELECOM;SWAN;SWAZI MTN;SWISSCOM MOBILE;SYRIATEL MOBILE TELECOM;T STAR TELECOM;T+ TELECOMUNICACOES;T-2;T-MOBILE AUSTRIA;T-MOBILE CROATIA;T-MOBILE CZECH REPUBLIC;T-MOBILE GERMANY;T-MOBILE HUNGARY;T-MOBILE MONTENEGRO;T-MOBILE NETHERLANDS;T-MOBILE ORANGE NETHERLANDS;T-MOBILE POLAND;T-MOBILE SLOVENSKO;T-MOBILE UNITED KINGDOM;T-MOBILE USA;TACOM TAJIKISTAN;TAIWAN MOBILE;TAIWAN MOBILE MOBITAI;TAIWAN MOBILE TRANSASIA;TALIYA GSM;TANGO LUXEMBURG;TANZANIA TELECOMMUNICATIONS;TASHI CELL;TATA MSPS TESTING DPC CHANGES;TATA TELESERVICES;TATA TELESERVICES SMS AGGREGATOR;TATA TELESERVICES SMS AGGREGATOR CDMA;TCC TONGA;TCELL SOMONCOM;TDC MOBIL NORWAY;TDC MOBIL SWEDEN;TE SA M ARGENTINA;TELALASKA NETWORKS;TELCELL;TELCOM MOBILE SOMALIA;TELE DANMARK NET MOBIL;TELE GREENLAND;TELE2 CROATIA;TELE2 EESTI;TELE2 LATVIA;TELE2 LITHUANIA;TELE2 NORGE;TELE2 RUSSIA ROSTOV CELLULAR;TELE2 SPRING MOBILE;TELE2 SVERIGE;TELE2NETHERLAND;TELECABLE;TELECEL BURKINA FASO;TELECEL CENTRAFRIQUE;TELECEL NIGER;TELECEL TELEFONICA CELULAR DEL PARAGUAY;TELECEL ZIMBABWE;TELECOM COOK ISLANDS;TELECOM DEVELOPMENT AFGHANISTAN COMPANY;TELECOM ITALIA MOBILE;TELECOM NAMIBIA;TELECOM NEW ZEALAND;TELECOM PERSONAL;TELECOM SEYCHELLES;TELECOM VANUATU;TELECOMMUNICATION KISH COMPANY;TELECOMUNICACIONES MOVILES DEL ECUADOR;TELEENA NETHERLANDS2;TELEENA UK;TELEFONICA 02 SLOVAKIA;TELEFONICA CELULAR CELTEL;TELEFONICA CELULAR DE BOLIVIA;TELEFONICA COMMUNICACIONES PERSONALES;TELEFONICA DEL PERU;TELEFONICA MOVIL DE CHILE;TELEFONICA MOVILES COLOMBIA;TELEFONICA MOVILES EL SALVADOR;TELEFONICA MOVILES ESPANA;TELEFONICA MOVILES GUATEMALA;TELEFONICA MOVILES MEXICO;TELEFONICA MOVILES MOVISTAR URUGUAY;TELEFONICA MOVILES NICARAGUA;TELEFONICA MOVILES PANAMASAMOVISTAR;TELEFONICA MOVILES VENEZUELA;TELEKOM SLOVENIJE;TELEKOM SRBIJA;TELEMACH MOBIL;TELEMETRIX TECHNOLOGIES;TELEMIG CELULAR VIVO MG BRAZIL;TELEMOVIL EL SALVADOR TIGO;TELENET;TELENOR;TELENOR MYANMAR;TELENOR NETWORK NORWAY;TELENOR NORWAY2;TELENOR PAKISTAN;TELENOR SWEDEN;TELENOR VODAFONE;TELESOM SOMALIA;TELESUR TELECOMMUNICARIEBEDRIJF SURINAME;TELESYSTEMS OF UKRAINE;TELETALK BANGLADESH;TELEWINGS COMMUNICATIONS SMS AGGREGATOR;TELIA MOBILE DENMARK;TELIASONERA FINLAND;TELIASONERA MOBILE NETWORKS;TELIN HONG KONG;TELKOM KENYA;TELKOM SOUTH AFRICA;TELKOMCEL EAST TIMOR;TELKOMSEL;TELMA TELECOM MALAGASY;TELMOB ONATEL;TELNA MOBILE USA;TELSTRA MOBILE;TELUS MOBILITY;TELUS MOBILITY 3G;TGBTESTANSIB;TGBTESTITUA;TGBTESTITUB;THE BAHAMAS TELECOMMUNICATION;THIRD KENTUCKY CELLULAR;THURAYA SATELLITE TELECOMMUNICATIONS;TIGO CELLTEL LANKA;TIGO RWANDA;TIGO SWEDEN;TIKIPHONE;TIM BRASIL;TIMOR TELECOM;TISMI;TM CELL TURKMENISTAN;TME OTECEL TELEFONICA MOVILES ECUADOR;TMN;TMP CORPORATION DBA SIMMETRY;TNM TELEKOM NETWORKS MALAWI;TOGO CELLULAIRE;TOT THAILAND;TRANSATEL;TRAVEL TELEKOMMUNIKATION;TRILOGY;TRIMOB;TRUPHONE;TSTT;TT MOBILE;TTSL ANDHRA PRADESH;TTSL BIHAR;TTSL DELHI;TTSL GUJARAT;TTSL HARYANA;TTSL HIMACHAL PRADESH;TTSL KARNATAKA;TTSL KERALA;TTSL KOLKATA;TTSL MADHYA PRADESH;TTSL MAHARASHTRA;TTSL MUMBAI;TTSL ORISSA;TTSL PUNJAB;TTSL RAJASTHAN;TTSL TAMILNADU;TTSL UTTAR PRADESH EAST;TTSL UTTAR PRADESH WEST;TTSL WEST BENGAL;TUNISIE TELECOM;TURK TELEKOM;TURKCELL;TWO DEGREES MOBILE;TYNTEC;U MOBILE MITV;UAB BITE GSM;UCOM ARMENIA;UCOM BURUNDI;UFONE PAK TELECOM MOBILE;UGANDA TELECOM;UKRANIAN RADIO SYSTEMS;UMNIAH MOBILE COMPANY;UNION TELEPHONE COMPANY;UNITARY ENTERPRISE VELCOM;UNITECH WIRELESS;UNITECH WIRELESS ANDHRA PRADESH;UNITECH WIRELESS BIHAR AND JHARKHAND;UNITECH WIRELESS GUJARAT;UNITECH WIRELESS MAHARASHTRA;UNITECH WIRELESS MUMBAI;UNITECH WIRELESS UTTAR PRADESH EAST;UNITECH WIRELESS UTTAR PRADESH WEST;UNITEL;UNITEL MONGOLIA;UNITEL SAO TOME AND PRINCIPE;UNITEL UZBEKISTAN;UNIVERSAL MOBILE SYSTEMS;UPC CABLECOM LGI MOBILE;UPC LGI MOBILE;US FIXED LINE DESTINATION;USAN GABON;UTS SETEL CURACAO ANTUT;UZMOBILE;VANU COVERAGE;VENTA MOBILE;VERIZON WIRELESS;VIDEOCON TELECOM SMS AGGREGATOR;VIDEOCON TELECOMMUNICATIONS;VIDEOTRON;VIETNAM MOBILE TELECOM SERVICES;VIETNAMOBILE;VIETTEL BURUNDI;VIETTEL CAMEROON;VIETTEL PERU;VIETTEL TANZANIA;VIETTEL TELECOM COMPANY;VIETTEL TIMOR;VIMPELCOM;VINAPHONE;VIP MOBILE;VIP OPERATOR;VIPNET;VITELCOM CELLULAR DBA INNOVATIVE WIRELES;VIVACEL KTELECOM;VIVACELL SOUTH SUDAN;VIVACELL SUDAN;VIVATEL BULGARIA;VIVO;VMOBILE CELTEL NIGERIA;VODACOM DRC;VODACOM MOZAMBIQUE;VODACOM TANZANIA;VODACOM1;VODACOM2;VODAFONE;VODAFONE ALBANIA;VODAFONE ANDHRA PRADESH;VODAFONE ASSAM;VODAFONE AUSTRALIA;VODAFONE BIHAR;VODAFONE CHENNAI;VODAFONE CYTA;VODAFONE CZECH REPUBLIC;VODAFONE D2;VODAFONE EGYPT;VODAFONE EGYPT1;VODAFONE ESSAR DELHI;VODAFONE ESSAR EAST;VODAFONE ESSAR GUJARAT;VODAFONE ESSAR KERALA;VODAFONE ESSAR MAHARASHTRA;VODAFONE ESSAR MUMBAI;VODAFONE ESSAR TAMIL NADU;VODAFONE FIJI;VODAFONE HARYANA;VODAFONE HIMACHAL PRADESH;VODAFONE HUNGARY;VODAFONE ICELAND;VODAFONE ICELAND1;VODAFONE INDIA SMS AGGREGATOR;VODAFONE IRELAND;VODAFONE JAMMU AND KASHMIR;VODAFONE KARNATAKA;VODAFONE KOLKATA;VODAFONE LIBERTEL HOLLAND;VODAFONE MADHYA PRADESH;VODAFONE MALTA;VODAFONE MARITIME MALTA;VODAFONE NETWORK;VODAFONE NEW ZEALAND;VODAFONE NORTH EAST;VODAFONE OMNITEL;VODAFONE ORISSA;VODAFONE PANAFON;VODAFONE PORTUGAL;VODAFONE PUNJAB;VODAFONE QATAR;VODAFONE RAJASTAN;VODAFONE ROMANIA;VODAFONE SPAIN;VODAFONE UA;VODAFONE UNITED KINGDOM;VODAFONE UP EAST;VODAFONE UP WEST;VODAFONE WEST BENGAL;VOICEWORKS;VRS M2M SERVICE;VTR MOVIL;WANA CORPORATE;WARID CONGO;WARID TELECOM1;WARID TELECOM2;WARID TELECOM3;WATANIYA NATIONAL MOBILE TELECOMMS;WATANIYA PALESTINE MOBILE;WATANIYA TELECOM ALGERIA;WAVE RUNNER CNMI;WEST CENTRAL WIRELESS;WIGHTMAN TELECOM;WIND;WIND HELLAS;WINS AERO;WIRELESS MAINGATE;WIRELS CONNECT;WOM CHILE 3G;WORLDFONE;XFERA SPAIN;XIT WIRELESS WATANIYA;XPRESS TELECOMMUNICATIONS;Y TELECOM;YEMEN MOBILE;YTL COMMUNICATIONS;YUBOTO;ZAIN;ZAIN BH MTC VODAFONE BAHRAIN;ZAIN COMMUNICATIONS GHANA;ZAIN FASTLIN MOBILE TELEPHONE SERVICES;ZAIN MOBITEL SUDAN;ZAIN MTC KUWAIT;ZAIN SOUTH SUDAN;ZANTEL ZANZIBAR TELECOM;ZAO SMARTS;</t>
+  </si>
+  <si>
+    <t>DT_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>DT_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>CP_InstanceLst_Val</t>
+  </si>
+  <si>
+    <t>CP_Account_Status</t>
+  </si>
+  <si>
+    <t>Test;Service;Terminated</t>
+  </si>
+  <si>
+    <t>Customer_Provisioning</t>
+  </si>
+  <si>
+    <t>Customer_Price_List_Emailer</t>
+  </si>
+  <si>
+    <t>CPLE_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>Customer_Price_Management</t>
+  </si>
+  <si>
+    <t>CPM_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>Product_Provisioning</t>
+  </si>
+  <si>
+    <t>PP_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>--Select--;MT SMS;MO SMS;Mobile LNS</t>
+  </si>
+  <si>
+    <t>PP_ProductStatusLst_Val</t>
+  </si>
+  <si>
+    <t>--Select--;Test;Service</t>
+  </si>
+  <si>
+    <t>PP_PriorityLst_Val</t>
+  </si>
+  <si>
+    <t>PP_CurrencyLst_Val</t>
+  </si>
+  <si>
+    <t>--Select--;AUD;CAD;EUR;GBP;INR;JPY;PLN;SGD;USD</t>
+  </si>
+  <si>
+    <t>Product_Coverage_Management</t>
+  </si>
+  <si>
+    <t>PCM_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>Product_Price_Management</t>
+  </si>
+  <si>
+    <t>PPM_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>Supplier_Provisioning</t>
+  </si>
+  <si>
+    <t>Supplier_Coverage_Management</t>
+  </si>
+  <si>
+    <t>Supplier_Cost_Management</t>
+  </si>
+  <si>
+    <t>Supplier_Destination_Cost</t>
+  </si>
+  <si>
+    <t>SP_InstanceLst</t>
+  </si>
+  <si>
+    <t>SP_AccountStatusLst</t>
+  </si>
+  <si>
+    <t>SDC_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>SDC_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>Number_Inventory</t>
+  </si>
+  <si>
+    <t>NI_TON</t>
+  </si>
+  <si>
+    <t>--Select--;SC;LN</t>
+  </si>
+  <si>
+    <t>NI_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>NI_StatusLst_Val</t>
+  </si>
+  <si>
+    <t>Product_Routing</t>
+  </si>
+  <si>
+    <t>Filtering_Rules</t>
+  </si>
+  <si>
+    <t>PR_CountryLst</t>
+  </si>
+  <si>
+    <t>FR_CountryLst</t>
+  </si>
+  <si>
+    <t>FR_DestinationLst</t>
+  </si>
+  <si>
+    <t>ALL;ACTIVE;INACTIVE;DELETED;EXPIRED</t>
+  </si>
+  <si>
+    <t>Delivery_Statistics_Uncorrelated</t>
+  </si>
+  <si>
+    <t>DSU_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>DSU_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>DSU_InstanceLst_Val</t>
+  </si>
+  <si>
+    <t>DSU_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>Delivery_Statistics</t>
+  </si>
+  <si>
+    <t>DS_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>DS_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>DS_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>DS_InstanceLst_Val</t>
+  </si>
+  <si>
+    <t>TopN_Destination</t>
+  </si>
+  <si>
+    <t>TND_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>TND_DestinationGranularityLst_Val</t>
+  </si>
+  <si>
+    <t>TND_SelectionBasedOnLst_Val</t>
+  </si>
+  <si>
+    <t>--Select--;Country;Destination</t>
+  </si>
+  <si>
+    <t>--Select--;Traffic;Revenue;Margin</t>
+  </si>
+  <si>
+    <t>Payable_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>Payable_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>Payable_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>Payable_BreakDownLst_Val</t>
+  </si>
+  <si>
+    <t>Date;Cost</t>
+  </si>
+  <si>
+    <t>Rerating</t>
+  </si>
+  <si>
+    <t>Rerating_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>RA_Daily_Report</t>
+  </si>
+  <si>
+    <t>RADR_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>RADR_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>RADR_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>SCovM_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>SCostM_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>Rerating_CountryLst_Val</t>
+  </si>
+  <si>
+    <t>Rerating_DestinationLst_Val</t>
+  </si>
+  <si>
+    <t>DT_ServiceLst_Val</t>
+  </si>
+  <si>
+    <t>ALL;SMSHUB-PREPROD-1;SMSHUB-PREPROD-2;SMSHUB-PREPROD-6;SMSHUB-PREPROD-7</t>
+  </si>
+  <si>
+    <t>--Select--;P1;P2</t>
+  </si>
+  <si>
+    <t>--Select--;ALL</t>
+  </si>
+  <si>
+    <t>--Select--;MT SMS</t>
+  </si>
+  <si>
+    <t>--Select--;MT SMS;MO SMS</t>
+  </si>
+  <si>
+    <t>--Select--;ABKHAZIA;AFGHANISTAN;ALBANIA;ALGERIA;AMERICAN SAMOA;ANDORRA;ANGOLA;ANGUILLA;ANTARCTICA;ANTIGUA &amp; BARB;ARGENTINA;ARMENIA;ARUBA;ASCENSION;AUSTRALIA;AUSTRIA;AZERBAIJAN;AZORES;BAHAMAS;BAHRAIN;BANGLADESH;BARBADOS;BARBUDA;BELARUS;BELGIUM;BELIZE;BENIN;BERMUDA;BHUTAN;BOLIVIA;BOSNIA-HERZEG.;BOTSWANA;BPOHUTHASWANA;BR VIRGIN ISL;BRAZIL;BRUNEI;BULGARIA;BURKINA FASO;BURUNDI;CAMBODIA;CAMEROON;CANADA;CAPE VERDE;CARRIACOU;CASEY;CAYMAN ISLANDS;CENTRAL AFRICA;CHAD;CHILE;CHINA;CHRISTMAS ISL.;CISKEI;COCOS ISLANDS;COLOMBIA;COMOROS;CONGO;COOK ISLANDS;COSTA RICA;COTE D IVOIRE;CROATIA;CUBA;CURAÇAO;CYPRUS;CYPRUS (NORTH);CZECH (REP);DAVIS;DEM REP CONGO;DENMARK;DIEGO GARCIA;DJIBOUTI;DOMINICA;DOMINICAN REP;EAST TIMOR;EASTER ISLAND;ECUADOR;EGYPT;EL SALVADOR;EQUA GUINEA;ERITREA;ESTONIA;ETHIOPIA;FALKLAND ISL.;FAROE ISLANDS;FIJI;FINLAND;FR. POLYNESIA;FRANCE;FRENCH ANTILLES;FRENCH GUIANA;GABON;GAMBIA;GEORGIA;GERMANY;GERMANY (EAST);GHANA;GIBRALTAR;GREECE;GREENLAND;GRENADA;GUADELOUPE;GUAM;GUATEMALA;GUERNSEY;GUINEA;GUINEA-BISSAU;GUYANA;HAITI;HONDURAS;HONG KONG;HUNGARY;ICELAND;INDIA;INDONESIA;IRAN;IRAQ;IRELAND;ISRAEL;ITALY;JAMAICA;JAPAN;JERSEY;JORDAN;KAZAKHSTAN;KENYA;KIRIBATI;KOSOVO;KUWAIT;KYRGYZSTAN;LAOS;LATVIA;LEBANON;LEEWARD;LESOTHO;LIBERIA;LIBYA;LIECHTENSTEIN;LITHUANIA;LUXEMBOURG;MACAU;MACEDONIA;MACQUARI;MADAGASCAR;MADEIRA;MALAWI;MALAYSIA;MALDIVES;MALI;MALTA;MARINA ISLANDS;MARSHALL ISLES;MARTINIQUE;MAURITANIA;MAURITIUS;MAWSON;MAYOTTE;MEXICO;MICRONESIA;MIDWAY ISLANDS;MOLDOVA;MONACO;MONGOLIA;MONTENEGRO;MONTSERRAT;MOROCCO;MOZAMBIQUE;MYANMAR;NAMIBIA;NAURU;NEPAL;NETH ANTILLES;NETHERLANDS;NEVIS;NEW CALEDONIA;NEW ZEALAND;NICARAGUA;NIGER;NIGERIA;NIUE ISLAND;NORFOLK ISLAND;NORTH KOREA;NORTH MARIANAS;NORWAY;OLD CNTRY ABBR;OMAN;PAKISTAN;PALAU;PALESTINE;PANAMA;PAPUA N.G.;PARAGUAY;PERU;PHILIPPINES;PITCAIRN ISLES;POLAND;PORTUGAL;PORTUGUESE GUIN;PORTUGUESE TIMO;PRINCIPE;PUERTO RICO;QATAR;REUNION;ROMANIA;RUSSIA;RWANDA;RYUKYU ISLAND;SAINT LUCIA;SAMOA;SAN MARINO;SAO TOME/PRINC.;SAUDI ARABIA;SENEGAL;SERBIA;SEYCHELLES;SIERRA LEONE;SINGAPORE;SINT MAARTEN;SLOVAKIA;SLOVENIA;SOLOMON ISLANDS;SOMALIA;SOUTH AFRICA;SOUTH KOREA;SOUTH SUDAN;SPAIN;SPANISH AFRICA;SRI LANKA;ST BARTHÉLEMY;ST HELENA;ST KITTS/NEVIS;ST VINCENT &amp; GR;ST-PIERRE-MIQ.;SUDAN;SURINAME;SWAZILAND;SWEDEN;SWITZERLAND;SYRIA;TAIWAN;TAJIKISTAN;TANZANIA;THAILAND;TOGO;TOKELAU;TONGA;TRANSKEI;TRINIDAD-TOBAGO;TUNISIA;TURKEY;TURKMENISTAN;TURKS &amp; CAICOS;TUVALU;UGANDA;UK;UKRAINE;UNIT. ARAB EMIR;UNITED STATES;URUGUAY;US VIRGIN  ISL;UZBEKISTAN;VANUATU;VATICAN CITY;VENEZUELA;VIETNAM;W INDIAN BRITIS;WAKE ISLAND;WALLIS &amp; FUTUNA;WESTERN SAHARA;WORLD WIDE;YEMEN (ARAB);YEMEN (DEMOC);ZAMBIA;ZIMBABWE</t>
+  </si>
+  <si>
+    <t>CP_Ins_InstanceStateLst_Val</t>
+  </si>
+  <si>
+    <t>CP_Traffic_TONBlacklistLst_Val</t>
+  </si>
+  <si>
+    <t>CP_Traffic_EnhancedDLRParameterLst_Val</t>
+  </si>
+  <si>
+    <t>CP_SMPP_SMPPVersionLst_Val</t>
+  </si>
+  <si>
+    <t>CP_SMPP_SMSCDefaultAlphabetLst_Val</t>
+  </si>
+  <si>
+    <t>CP_SMPP_MsgIDTypeLst_Val</t>
+  </si>
+  <si>
+    <t>CP_SMPP_MsgIDLengthLst_Val</t>
+  </si>
+  <si>
+    <t>CP_SMPP_DataCodingSupportedLst_Val</t>
+  </si>
+  <si>
+    <t>CP_SMPP_EnhancedDLRFormatLst_Val</t>
+  </si>
+  <si>
+    <t>Active;Inactive</t>
+  </si>
+  <si>
+    <t>Alphanumeric (5);MSISDN (1);Shortcode (2)</t>
+  </si>
+  <si>
+    <t>Initial Destination Carrier (1);Final Destination Carrier (2);Portability Flag (3);Price for Termination - Currency (4)</t>
+  </si>
+  <si>
+    <t>3.4;3.3</t>
+  </si>
+  <si>
+    <t>GSM 7bits;ASCII;Latin 1;UCS2</t>
+  </si>
+  <si>
+    <t>--Select--;String;Hex;Decimal</t>
+  </si>
+  <si>
+    <t>--Select--;9;33;65</t>
+  </si>
+  <si>
+    <t>GSM 7bits;GSM 8bits;ASCII;Latin 1;UCS 2</t>
+  </si>
+  <si>
+    <t>Short Message + TLVs (1);Short message (2);TLVs Only (3)</t>
+  </si>
+  <si>
+    <t>SP_Traffic_OASenderTypeSupportLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_SMPPVersionLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_DLRSupportLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_MsgIDTypeLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_MsgIDLengthLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_SMSCDefaultAlphabetLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_SMSCMsgModeLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SMPP_DataCodingSupportedLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SS7_SM_RP_PRIFlagLst_Val</t>
+  </si>
+  <si>
+    <t>SP_SS7_MTDCSSupportLst_Val</t>
+  </si>
+  <si>
+    <t>SP_HTTP_DLRSupportLst_Val</t>
+  </si>
+  <si>
+    <t>SP_Ins_InstanceStateLst_Val</t>
+  </si>
+  <si>
+    <t>Alphanumeric;MSISDN;Shortcode</t>
+  </si>
+  <si>
+    <t>Yes;No</t>
+  </si>
+  <si>
+    <t>--Select--;String;Decimal;Hex-Decimal (submit_sm_resp-Deliver_sm);Decimal-Hex (submit_sm_resp-Deliver_sm);Hex</t>
+  </si>
+  <si>
+    <t>Store;Datagram</t>
+  </si>
+  <si>
+    <t>1;0</t>
+  </si>
+  <si>
+    <t>GSM 7 bit;GSM 8 bits;UCS 2;Binary</t>
+  </si>
+  <si>
+    <t>Normal User - 
+Validate options from fixed dropdowns</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +3248,7 @@
     <numFmt numFmtId="166" formatCode="[$-14009]d\.m\.yy;@"/>
     <numFmt numFmtId="167" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3046,8 +3402,30 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3138,6 +3516,96 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -3213,7 +3681,7 @@
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="165"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="102">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyAlignment="1" applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
@@ -3316,6 +3784,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="4"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="16" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="17" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="19" fontId="22" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="23" fontId="23" numFmtId="164" xfId="2"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="21" fontId="23" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="20" fontId="23" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="24" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="22" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="21" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="25" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="18" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="20" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="23" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="26" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="19" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="24" fontId="23" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="27" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="29" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="28" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="30" fontId="20" numFmtId="164" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="13" fontId="12" numFmtId="164" xfId="5">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
@@ -3634,7 +4126,7 @@
   <dimension ref="A1:BL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10738,7 +11230,7 @@
   <dimension ref="A1:BS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11288,13 +11780,809 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:DK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="11.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="19" max="20" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="35" max="36" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="42" max="43" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="58" max="64" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="70" max="71" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="74" max="74" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="75" max="76" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="77" max="77" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="78" max="78" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="79" max="79" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="80" max="80" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="81" max="81" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="82" max="82" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="83" max="83" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="84" max="84" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="85" max="88" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="89" max="89" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="90" max="93" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="94" max="94" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="95" max="95" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="96" max="97" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="98" max="98" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="99" max="99" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="100" max="100" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="101" max="101" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="102" max="102" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="103" max="103" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="104" max="104" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="105" max="105" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="106" max="106" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="107" max="107" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="109" max="109" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="110" max="110" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="111" max="111" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="112" max="112" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="113" max="113" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="114" max="114" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="115" max="115" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="15.75" r="1" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="84" t="s">
+        <v>783</v>
+      </c>
+      <c r="J1" s="55" t="s">
+        <v>784</v>
+      </c>
+      <c r="K1" s="55" t="s">
+        <v>786</v>
+      </c>
+      <c r="L1" s="55" t="s">
+        <v>792</v>
+      </c>
+      <c r="M1" s="56" t="s">
+        <v>795</v>
+      </c>
+      <c r="N1" s="56" t="s">
+        <v>797</v>
+      </c>
+      <c r="O1" s="56" t="s">
+        <v>801</v>
+      </c>
+      <c r="P1" s="56" t="s">
+        <v>807</v>
+      </c>
+      <c r="Q1" s="56" t="s">
+        <v>913</v>
+      </c>
+      <c r="R1" s="80" t="s">
+        <v>861</v>
+      </c>
+      <c r="S1" s="80" t="s">
+        <v>989</v>
+      </c>
+      <c r="T1" s="80" t="s">
+        <v>917</v>
+      </c>
+      <c r="U1" s="80" t="s">
+        <v>918</v>
+      </c>
+      <c r="V1" s="83" t="s">
+        <v>340</v>
+      </c>
+      <c r="W1" s="56" t="s">
+        <v>922</v>
+      </c>
+      <c r="X1" s="56" t="s">
+        <v>919</v>
+      </c>
+      <c r="Y1" s="56" t="s">
+        <v>920</v>
+      </c>
+      <c r="Z1" s="56" t="s">
+        <v>996</v>
+      </c>
+      <c r="AA1" s="56" t="s">
+        <v>997</v>
+      </c>
+      <c r="AB1" s="56" t="s">
+        <v>998</v>
+      </c>
+      <c r="AC1" s="56" t="s">
+        <v>999</v>
+      </c>
+      <c r="AD1" s="56" t="s">
+        <v>1000</v>
+      </c>
+      <c r="AE1" s="56" t="s">
+        <v>1001</v>
+      </c>
+      <c r="AF1" s="56" t="s">
+        <v>1002</v>
+      </c>
+      <c r="AG1" s="56" t="s">
+        <v>1003</v>
+      </c>
+      <c r="AH1" s="56" t="s">
+        <v>1004</v>
+      </c>
+      <c r="AI1" s="81" t="s">
+        <v>923</v>
+      </c>
+      <c r="AJ1" s="81" t="s">
+        <v>924</v>
+      </c>
+      <c r="AK1" s="58" t="s">
+        <v>925</v>
+      </c>
+      <c r="AL1" s="58" t="s">
+        <v>926</v>
+      </c>
+      <c r="AM1" s="86" t="s">
+        <v>864</v>
+      </c>
+      <c r="AN1" s="91" t="s">
+        <v>927</v>
+      </c>
+      <c r="AO1" s="91" t="s">
+        <v>928</v>
+      </c>
+      <c r="AP1" s="91" t="s">
+        <v>930</v>
+      </c>
+      <c r="AQ1" s="91" t="s">
+        <v>933</v>
+      </c>
+      <c r="AR1" s="91" t="s">
+        <v>932</v>
+      </c>
+      <c r="AS1" s="87" t="s">
+        <v>935</v>
+      </c>
+      <c r="AT1" s="87" t="s">
+        <v>936</v>
+      </c>
+      <c r="AU1" s="87" t="s">
+        <v>937</v>
+      </c>
+      <c r="AV1" s="87" t="s">
+        <v>938</v>
+      </c>
+      <c r="AW1" s="82" t="s">
+        <v>337</v>
+      </c>
+      <c r="AX1" s="93" t="s">
+        <v>939</v>
+      </c>
+      <c r="AY1" s="93" t="s">
+        <v>943</v>
+      </c>
+      <c r="AZ1" s="93" t="s">
+        <v>944</v>
+      </c>
+      <c r="BA1" s="93" t="s">
+        <v>1025</v>
+      </c>
+      <c r="BB1" s="93" t="s">
+        <v>1014</v>
+      </c>
+      <c r="BC1" s="93" t="s">
+        <v>1015</v>
+      </c>
+      <c r="BD1" s="93" t="s">
+        <v>1016</v>
+      </c>
+      <c r="BE1" s="93" t="s">
+        <v>1017</v>
+      </c>
+      <c r="BF1" s="93" t="s">
+        <v>1018</v>
+      </c>
+      <c r="BG1" s="93" t="s">
+        <v>1019</v>
+      </c>
+      <c r="BH1" s="93" t="s">
+        <v>1020</v>
+      </c>
+      <c r="BI1" s="93" t="s">
+        <v>1021</v>
+      </c>
+      <c r="BJ1" s="93" t="s">
+        <v>1022</v>
+      </c>
+      <c r="BK1" s="93" t="s">
+        <v>1023</v>
+      </c>
+      <c r="BL1" s="93" t="s">
+        <v>1024</v>
+      </c>
+      <c r="BM1" s="89" t="s">
+        <v>940</v>
+      </c>
+      <c r="BN1" s="89" t="s">
+        <v>985</v>
+      </c>
+      <c r="BO1" s="94" t="s">
+        <v>941</v>
+      </c>
+      <c r="BP1" s="94" t="s">
+        <v>986</v>
+      </c>
+      <c r="BQ1" s="95" t="s">
+        <v>942</v>
+      </c>
+      <c r="BR1" s="95" t="s">
+        <v>945</v>
+      </c>
+      <c r="BS1" s="95" t="s">
+        <v>946</v>
+      </c>
+      <c r="BT1" s="83" t="s">
+        <v>869</v>
+      </c>
+      <c r="BU1" s="81" t="s">
+        <v>947</v>
+      </c>
+      <c r="BV1" s="81" t="s">
+        <v>948</v>
+      </c>
+      <c r="BW1" s="81" t="s">
+        <v>950</v>
+      </c>
+      <c r="BX1" s="81" t="s">
+        <v>951</v>
+      </c>
+      <c r="BY1" s="86" t="s">
+        <v>871</v>
+      </c>
+      <c r="BZ1" s="88" t="s">
+        <v>952</v>
+      </c>
+      <c r="CA1" s="88" t="s">
+        <v>954</v>
+      </c>
+      <c r="CB1" s="98" t="s">
+        <v>953</v>
+      </c>
+      <c r="CC1" s="98" t="s">
+        <v>955</v>
+      </c>
+      <c r="CD1" s="98" t="s">
+        <v>956</v>
+      </c>
+      <c r="CE1" s="96" t="s">
+        <v>835</v>
+      </c>
+      <c r="CF1" s="99" t="s">
+        <v>958</v>
+      </c>
+      <c r="CG1" s="99" t="s">
+        <v>959</v>
+      </c>
+      <c r="CH1" s="99" t="s">
+        <v>960</v>
+      </c>
+      <c r="CI1" s="99" t="s">
+        <v>962</v>
+      </c>
+      <c r="CJ1" s="99" t="s">
+        <v>961</v>
+      </c>
+      <c r="CK1" s="97" t="s">
+        <v>963</v>
+      </c>
+      <c r="CL1" s="97" t="s">
+        <v>964</v>
+      </c>
+      <c r="CM1" s="97" t="s">
+        <v>965</v>
+      </c>
+      <c r="CN1" s="97" t="s">
+        <v>966</v>
+      </c>
+      <c r="CO1" s="97" t="s">
+        <v>967</v>
+      </c>
+      <c r="CP1" s="90" t="s">
+        <v>968</v>
+      </c>
+      <c r="CQ1" s="90" t="s">
+        <v>969</v>
+      </c>
+      <c r="CR1" s="90" t="s">
+        <v>970</v>
+      </c>
+      <c r="CS1" s="90" t="s">
+        <v>971</v>
+      </c>
+      <c r="CT1" s="85" t="s">
+        <v>822</v>
+      </c>
+      <c r="CU1" s="100" t="s">
+        <v>823</v>
+      </c>
+      <c r="CV1" s="100" t="s">
+        <v>825</v>
+      </c>
+      <c r="CW1" s="100" t="s">
+        <v>831</v>
+      </c>
+      <c r="CX1" s="100" t="s">
+        <v>833</v>
+      </c>
+      <c r="CY1" s="90" t="s">
+        <v>873</v>
+      </c>
+      <c r="CZ1" s="90" t="s">
+        <v>974</v>
+      </c>
+      <c r="DA1" s="90" t="s">
+        <v>975</v>
+      </c>
+      <c r="DB1" s="90" t="s">
+        <v>976</v>
+      </c>
+      <c r="DC1" s="90" t="s">
+        <v>977</v>
+      </c>
+      <c r="DD1" s="92" t="s">
+        <v>979</v>
+      </c>
+      <c r="DE1" s="92" t="s">
+        <v>980</v>
+      </c>
+      <c r="DF1" s="92" t="s">
+        <v>987</v>
+      </c>
+      <c r="DG1" s="92" t="s">
+        <v>988</v>
+      </c>
+      <c r="DH1" s="80" t="s">
+        <v>981</v>
+      </c>
+      <c r="DI1" s="80" t="s">
+        <v>982</v>
+      </c>
+      <c r="DJ1" s="80" t="s">
+        <v>983</v>
+      </c>
+      <c r="DK1" s="80" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row ht="45" r="2" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" t="s">
+        <v>846</v>
+      </c>
+      <c r="J2" t="s">
+        <v>846</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="L2" t="s">
+        <v>915</v>
+      </c>
+      <c r="M2" t="s">
+        <v>846</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="O2" t="s">
+        <v>915</v>
+      </c>
+      <c r="P2" t="s">
+        <v>916</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>914</v>
+      </c>
+      <c r="R2" t="s">
+        <v>846</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="T2" t="s">
+        <v>915</v>
+      </c>
+      <c r="U2" t="s">
+        <v>916</v>
+      </c>
+      <c r="V2" t="s">
+        <v>846</v>
+      </c>
+      <c r="W2" t="s">
+        <v>846</v>
+      </c>
+      <c r="X2" t="s">
+        <v>990</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>921</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AJ2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AO2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="AP2" s="21" t="s">
+        <v>931</v>
+      </c>
+      <c r="AQ2" s="21" t="s">
+        <v>934</v>
+      </c>
+      <c r="AR2" s="21" t="s">
+        <v>991</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AT2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AV2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>846</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>990</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>921</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>846</v>
+      </c>
+      <c r="BN2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>846</v>
+      </c>
+      <c r="BP2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>855</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>915</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>916</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>671</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>671</v>
+      </c>
+      <c r="BV2" s="21" t="s">
+        <v>949</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>995</v>
+      </c>
+      <c r="BX2" s="21" t="s">
+        <v>957</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>671</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CA2" s="21" t="s">
+        <v>992</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>915</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CG2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>915</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>916</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>914</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CL2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>915</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>916</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>914</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CQ2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="CR2" s="21" t="s">
+        <v>972</v>
+      </c>
+      <c r="CS2" s="21" t="s">
+        <v>973</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CV2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>671</v>
+      </c>
+      <c r="CZ2" s="21" t="s">
+        <v>929</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>28</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>978</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>671</v>
+      </c>
+      <c r="DE2" s="21" t="s">
+        <v>993</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>28</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>28</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>671</v>
+      </c>
+      <c r="DI2" s="21" t="s">
+        <v>994</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>28</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E2"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11323,6 +12611,18 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -14063,8 +15363,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14360,12 +15660,8 @@
       <c r="G5" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>913</v>
-      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
         <v>32</v>
       </c>
@@ -14442,12 +15738,8 @@
       <c r="G6" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>914</v>
-      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
         <v>32</v>
       </c>
@@ -14670,9 +15962,7 @@
       <c r="G9" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Filtering Rules screen automation scripts are added
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -1,46 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="22" firstSheet="20" tabRatio="855" windowHeight="7755" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="855" firstSheet="21" activeTab="27"/>
   </bookViews>
   <sheets>
-    <sheet name="Customer_Provisioning_Screen" r:id="rId1" sheetId="24"/>
-    <sheet name="Custom_Error" r:id="rId2" sheetId="27"/>
-    <sheet name="Supplier_Provisioning_Screen" r:id="rId3" sheetId="1"/>
-    <sheet name="Number_Inventory_Screen" r:id="rId4" sheetId="2"/>
-    <sheet name="Supplier_Cost_Management_Screen" r:id="rId5" sheetId="3"/>
-    <sheet name="Supplier_Coverage_Screen" r:id="rId6" sheetId="4"/>
-    <sheet name="MNP_Screen" r:id="rId7" sheetId="25"/>
-    <sheet name="Product_Provisioning_Screen" r:id="rId8" sheetId="5"/>
-    <sheet name="Customer_PriceManagement_Screen" r:id="rId9" sheetId="6"/>
-    <sheet name="Product_Coverage_Screen" r:id="rId10" sheetId="8"/>
-    <sheet name="Product_Routing_Screen" r:id="rId11" sheetId="10"/>
-    <sheet name="Delivery_Statistics_Screen" r:id="rId12" sheetId="17"/>
-    <sheet name="Payable_Screen" r:id="rId13" sheetId="20"/>
-    <sheet name="RADailyReport_Screen" r:id="rId14" sheetId="22"/>
-    <sheet name="Receivables_Screen" r:id="rId15" sheetId="18"/>
-    <sheet name="Product_Default" r:id="rId16" sheetId="26"/>
-    <sheet name="Product_Price_Management_Screen" r:id="rId17" sheetId="11"/>
-    <sheet name="Destination_Trend" r:id="rId18" sheetId="21"/>
-    <sheet name="Performance_Trend" r:id="rId19" sheetId="12"/>
-    <sheet name="Checking_Roles_Access" r:id="rId20" sheetId="13"/>
-    <sheet name="Customer_Coverage_Screen" r:id="rId21" sheetId="7"/>
-    <sheet name="ValidatingFields_Roles" r:id="rId22" sheetId="14"/>
-    <sheet name="ValidatingOptions_FixedDropdown" r:id="rId23" sheetId="31"/>
-    <sheet name="ScreenAccessBasedOnRoles" r:id="rId24" sheetId="15"/>
-    <sheet name="Custom_Error_Screen" r:id="rId25" sheetId="28"/>
-    <sheet name="XML_Comparison" r:id="rId26" sheetId="29"/>
-    <sheet name="RetryScheme" r:id="rId27" sheetId="30"/>
+    <sheet name="Customer_Provisioning_Screen" sheetId="24" r:id="rId1"/>
+    <sheet name="Custom_Error" sheetId="27" r:id="rId2"/>
+    <sheet name="Supplier_Provisioning_Screen" sheetId="1" r:id="rId3"/>
+    <sheet name="Number_Inventory_Screen" sheetId="2" r:id="rId4"/>
+    <sheet name="Supplier_Cost_Management_Screen" sheetId="3" r:id="rId5"/>
+    <sheet name="Supplier_Coverage_Screen" sheetId="4" r:id="rId6"/>
+    <sheet name="MNP_Screen" sheetId="25" r:id="rId7"/>
+    <sheet name="Product_Provisioning_Screen" sheetId="5" r:id="rId8"/>
+    <sheet name="Customer_PriceManagement_Screen" sheetId="6" r:id="rId9"/>
+    <sheet name="Product_Coverage_Screen" sheetId="8" r:id="rId10"/>
+    <sheet name="Product_Routing_Screen" sheetId="10" r:id="rId11"/>
+    <sheet name="Delivery_Statistics_Screen" sheetId="17" r:id="rId12"/>
+    <sheet name="Payable_Screen" sheetId="20" r:id="rId13"/>
+    <sheet name="RADailyReport_Screen" sheetId="22" r:id="rId14"/>
+    <sheet name="Receivables_Screen" sheetId="18" r:id="rId15"/>
+    <sheet name="Product_Default" sheetId="26" r:id="rId16"/>
+    <sheet name="Product_Price_Management_Screen" sheetId="11" r:id="rId17"/>
+    <sheet name="Destination_Trend" sheetId="21" r:id="rId18"/>
+    <sheet name="Performance_Trend" sheetId="12" r:id="rId19"/>
+    <sheet name="Checking_Roles_Access" sheetId="13" r:id="rId20"/>
+    <sheet name="Customer_Coverage_Screen" sheetId="7" r:id="rId21"/>
+    <sheet name="ValidatingFields_Roles" sheetId="14" r:id="rId22"/>
+    <sheet name="ValidatingOptions_FixedDropdown" sheetId="31" r:id="rId23"/>
+    <sheet name="ScreenAccessBasedOnRoles" sheetId="15" r:id="rId24"/>
+    <sheet name="Custom_Error_Screen" sheetId="28" r:id="rId25"/>
+    <sheet name="XML_Comparison" sheetId="29" r:id="rId26"/>
+    <sheet name="RetryScheme" sheetId="30" r:id="rId27"/>
+    <sheet name="FilteringRules" sheetId="33" r:id="rId28"/>
+    <sheet name="Referance" sheetId="34" r:id="rId29"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3605" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3757" uniqueCount="1070">
   <si>
     <t>Username</t>
   </si>
@@ -3236,6 +3238,194 @@
   <si>
     <t>Normal User - 
 Validate options from fixed dropdowns</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>CustomerAccountName</t>
+  </si>
+  <si>
+    <t>SupplierName</t>
+  </si>
+  <si>
+    <t>TON_BL_Cond</t>
+  </si>
+  <si>
+    <t>OA_BL_Cond</t>
+  </si>
+  <si>
+    <t>OA_PassThrough</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>RuleID_Filter</t>
+  </si>
+  <si>
+    <t>OA_Filter</t>
+  </si>
+  <si>
+    <t>Routing&gt;Filtering Rules</t>
+  </si>
+  <si>
+    <t>SubRules_Json</t>
+  </si>
+  <si>
+    <t>ALGERIA</t>
+  </si>
+  <si>
+    <t>ALGERIE TELECOM MOBILE</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>comment123</t>
+  </si>
+  <si>
+    <t>ZEN INTERACTIVE TECHNOLOGIES</t>
+  </si>
+  <si>
+    <t>UI Fileds validation</t>
+  </si>
+  <si>
+    <t>Create a new rule and subrule</t>
+  </si>
+  <si>
+    <t>Edit a rule</t>
+  </si>
+  <si>
+    <t>RuleID</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "OA_Cond": "123",
+    "TON_Cond": "LN(1)",
+    "OA_Result": "1234",
+    "TON_Result": "AN(5)",
+    "Status": "D"
+  }
+]</t>
+  </si>
+  <si>
+    <t>FilteringRules</t>
+  </si>
+  <si>
+    <t>SubRules_Json ( new Rule )</t>
+  </si>
+  <si>
+    <t>SubRules_Json ( edit Rule )</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "ChangeType": "Edit",
+    "OA_Cond": "123",
+    "OA_Cond_New": "123",
+    "TON_Cond": "LN(1)",
+    "TON_Cond_New": "LN(1)",
+    "OA_Result": "1234",
+    "OA_Result_New": "1234",
+    "TON_Result": "AN(5)",
+    "TON_Result_New": "AN(5)",
+    "Status": "D"
+  },
+  {
+    "ChangeType": "Add",
+    "OA_Cond": "123",
+    "TON_Cond": "LN(1)",
+    "OA_Result": "1234",
+    "TON_Result": "AN(5)",
+    "Status": "D"
+  },
+  {
+    "ChangeType": "Delete",
+    "OA_Cond": "123",
+    "TON_Cond": "LN(1)",
+    "OA_Result": "1234",
+    "TON_Result": "AN(5)"
+  },
+  {
+    "ChangeType": "StatusChange",
+    "OA_Cond": "123",
+    "TON_Cond": "LN(1)",
+    "OA_Result": "1234",
+    "TON_Result": "AN(5)",
+    "Status": "D"
+  }
+]</t>
+  </si>
+  <si>
+    <t>[
+ {
+    "ChangeType": "Delete",
+    "OA_Cond": "123",
+    "TON_Cond": "LN(1)",
+    "OA_Result": "1234",
+    "TON_Result": "AN(5)"
+  }
+]</t>
+  </si>
+  <si>
+    <t>Delete a rule</t>
+  </si>
+  <si>
+    <t>Popup Validation</t>
+  </si>
+  <si>
+    <t>CSVExportValidation</t>
+  </si>
+  <si>
+    <t>RuleIDLog</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "User": "sidhajyoti.mishra@tatacommunications.com",
+    "Date": "07/31/2017 06:10:44",
+    "Active": "No",
+    "PushedToHubs": "No"
+  },
+  {
+    "User": "sidhajyoti.mishra@tatacommunications.com",
+    "Date": "07/31/2017 06:12:55",
+    "Active": "Yes",
+    "PushedToHubs": "No"
+  },
+  {
+    "User": "sidhajyoti.mishra@tatacommunications.com",
+    "Date": "07/31/2017 07:33:20",
+    "Active": "No",
+    "PushedToHubs": "No"
+  },
+  {
+    "User": "sonali.das@tatacommunications.com",
+    "Date": "08/01/2017 07:03:20",
+    "Active": "Yes",
+    "PushedToHubs": "Yes"
+  }
+]</t>
+  </si>
+  <si>
+    <t>OALinksValidation</t>
+  </si>
+  <si>
+    <t>ValidateNoDuplicatesInSubRuleRows</t>
+  </si>
+  <si>
+    <t>RuleIDLinkValidation</t>
   </si>
 </sst>
 </file>
@@ -3662,152 +3852,158 @@
     </border>
   </borders>
   <cellStyleXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="165"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="14" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
+  <cellXfs count="106">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="11" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="11" numFmtId="49" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="14" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="11" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="11" numFmtId="3" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="167" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="5" fontId="3" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="17" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="12" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="12" numFmtId="3" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="167" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="9" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="10" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="11" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="12" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="12" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="13" fontId="12" numFmtId="164" xfId="5">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="20" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="12" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="12" fillId="13" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="5"/>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="6" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="8" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="3" fillId="10" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="3" fillId="12" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="6" fontId="21" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="3" fillId="14" fontId="12" numFmtId="164" xfId="2">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="12" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyProtection="1" borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="14" fontId="12" numFmtId="164" xfId="5">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="3" fillId="0" fontId="14" numFmtId="164" xfId="4"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="12" numFmtId="164" xfId="5"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="13" numFmtId="0" xfId="3"/>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="15" fontId="12" numFmtId="164" xfId="5"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="13" fontId="12" numFmtId="164" xfId="5">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="15" borderId="3" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="13" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="4"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="16" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="17" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="19" fontId="22" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="23" fontId="23" numFmtId="164" xfId="2"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="24" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="21" fontId="23" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="20" fontId="23" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="24" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="22" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="21" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="25" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="18" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="20" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="23" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="26" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="19" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="24" fontId="23" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="27" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="29" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="28" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="2" fillId="30" fontId="20" numFmtId="164" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="13" fontId="12" numFmtId="164" xfId="5">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="16" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="17" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="22" fillId="19" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="23" fillId="23" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="23" fillId="21" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="23" fillId="20" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="24" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="22" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="21" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="25" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="18" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="20" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="23" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="26" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="19" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="23" fillId="24" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="27" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="29" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="28" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="20" fillId="30" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="12" fillId="13" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
@@ -3816,14 +4012,14 @@
     <cellStyle name="Excel Built-in Normal 2" xfId="5"/>
     <cellStyle name="Heading" xfId="7"/>
     <cellStyle name="Heading1" xfId="8"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Result" xfId="9"/>
     <cellStyle name="Result2" xfId="10"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3840,10 +4036,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3878,7 +4074,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3913,7 +4109,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4001,7 +4197,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -4010,13 +4206,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -4026,7 +4222,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -4035,7 +4231,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -4044,7 +4240,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -4054,12 +4250,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -4090,7 +4286,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -4109,7 +4305,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -4121,7 +4317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BL10"/>
   <sheetViews>
@@ -4131,66 +4327,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="18" max="19" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="22" max="23" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="36" max="37" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="38" max="39" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="50" max="50" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="60" max="60" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="62" max="62" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="20" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="25" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -4426,7 +4622,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row customHeight="1" ht="17.25" r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -4482,7 +4678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -4527,7 +4723,7 @@
         <v>26</v>
       </c>
     </row>
-    <row ht="15.75" r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -4574,7 +4770,7 @@
         <v>579</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -4630,7 +4826,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -4668,7 +4864,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row ht="15.75" r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -4733,7 +4929,7 @@
         <v>584</v>
       </c>
     </row>
-    <row ht="15.75" r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -4886,30 +5082,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3:F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F8"/>
-    <hyperlink r:id="rId7" ref="BA5"/>
-    <hyperlink r:id="rId8" ref="E2"/>
-    <hyperlink r:id="rId9" ref="E3"/>
-    <hyperlink r:id="rId10" ref="E4"/>
-    <hyperlink r:id="rId11" ref="E5"/>
-    <hyperlink r:id="rId12" ref="E6"/>
-    <hyperlink r:id="rId13" ref="E7"/>
-    <hyperlink r:id="rId14" ref="E8"/>
-    <hyperlink r:id="rId15" ref="E9"/>
-    <hyperlink r:id="rId16" ref="E10"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="BA5" r:id="rId7"/>
+    <hyperlink ref="E2" r:id="rId8"/>
+    <hyperlink ref="E3" r:id="rId9"/>
+    <hyperlink ref="E4" r:id="rId10"/>
+    <hyperlink ref="E5" r:id="rId11"/>
+    <hyperlink ref="E6" r:id="rId12"/>
+    <hyperlink ref="E7" r:id="rId13"/>
+    <hyperlink ref="E8" r:id="rId14"/>
+    <hyperlink ref="E9" r:id="rId15"/>
+    <hyperlink ref="E10" r:id="rId16"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AB7"/>
   <sheetViews>
@@ -4919,37 +5115,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="46.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="3.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="3.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
@@ -5399,31 +5595,31 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="Z2:AB7" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:AB7">
       <formula1>"ON,OFF"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F2"/>
-    <hyperlink r:id="rId7" ref="E2"/>
-    <hyperlink r:id="rId8" ref="E3"/>
-    <hyperlink r:id="rId9" ref="E4"/>
-    <hyperlink r:id="rId10" ref="E5"/>
-    <hyperlink r:id="rId11" ref="E6"/>
-    <hyperlink r:id="rId12" ref="E7"/>
+    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="E2" r:id="rId7"/>
+    <hyperlink ref="E3" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId12"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:P8"/>
   <sheetViews>
@@ -5433,25 +5629,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="103.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="103.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>259</v>
       </c>
@@ -5588,7 +5784,7 @@
         <v>149</v>
       </c>
     </row>
-    <row ht="30" r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -5816,21 +6012,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F8"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId8" ref="E2:E8"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AA10"/>
   <sheetViews>
@@ -5840,31 +6036,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="11" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="134.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="134.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -6562,32 +6758,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F5"/>
-    <hyperlink r:id="rId7" ref="E2"/>
-    <hyperlink r:id="rId8" ref="E3"/>
-    <hyperlink r:id="rId9" ref="E4"/>
-    <hyperlink r:id="rId10" ref="E5"/>
-    <hyperlink r:id="rId11" ref="E6"/>
-    <hyperlink r:id="rId12" ref="E7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId13" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId14" ref="F9"/>
-    <hyperlink display="Newtglobal@123" r:id="rId15" ref="F10"/>
-    <hyperlink r:id="rId16" ref="E8"/>
-    <hyperlink r:id="rId17" ref="E9"/>
-    <hyperlink r:id="rId18" ref="E10"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="E2" r:id="rId7"/>
+    <hyperlink ref="E3" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId12"/>
+    <hyperlink ref="F8" r:id="rId13" display="Newtglobal@123"/>
+    <hyperlink ref="F9" r:id="rId14" display="Newtglobal@123"/>
+    <hyperlink ref="F10" r:id="rId15" display="Newtglobal@123"/>
+    <hyperlink ref="E8" r:id="rId16"/>
+    <hyperlink ref="E9" r:id="rId17"/>
+    <hyperlink ref="E10" r:id="rId18"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AE8"/>
   <sheetViews>
@@ -6597,35 +6793,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="71.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="42.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -7163,25 +7359,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F4"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId8" ref="E2:E8"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="AA8:AE8 AE7 X8 AA7:AD7"/>
+    <ignoredError sqref="AA8:AE8 AE7 X8 AA7:AD7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AG11"/>
   <sheetViews>
@@ -7191,37 +7387,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="71.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="42.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -7793,63 +7989,63 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F4"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId8" ref="E2:E8"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="X8 AE8:AF8 AA8:AC8 AB7 AD7:AE7 AG7"/>
+    <ignoredError sqref="X8 AE8:AF8 AA8:AC8 AB7 AD7:AE7 AG7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="71.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="42.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="42.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -8392,32 +8588,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F4"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId8" ref="E2:E8"/>
-    <hyperlink r:id="rId9" ref="D2"/>
-    <hyperlink r:id="rId10" ref="D3"/>
-    <hyperlink r:id="rId11" ref="D4"/>
-    <hyperlink r:id="rId12" ref="D5"/>
-    <hyperlink r:id="rId13" ref="D6"/>
-    <hyperlink r:id="rId14" ref="D7"/>
-    <hyperlink r:id="rId15" ref="D8"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="D2" r:id="rId9"/>
+    <hyperlink ref="D3" r:id="rId10"/>
+    <hyperlink ref="D4" r:id="rId11"/>
+    <hyperlink ref="D5" r:id="rId12"/>
+    <hyperlink ref="D6" r:id="rId13"/>
+    <hyperlink ref="D7" r:id="rId14"/>
+    <hyperlink ref="D8" r:id="rId15"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId16"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="AB7:AC8 AE7:AE8 X8:Y8"/>
+    <ignoredError sqref="AB7:AC8 AE7:AE8 X8:Y8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8528,7 +8724,7 @@
         <v>183</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -8561,7 +8757,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row ht="15.75" r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -8629,7 +8825,7 @@
         <v>625</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -8691,7 +8887,7 @@
       </c>
       <c r="AH4" s="39"/>
     </row>
-    <row ht="15.75" r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -8729,7 +8925,7 @@
         <v>647</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -8798,7 +8994,7 @@
         <v>622</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -8851,132 +9047,132 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="20" max="21" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="28" max="29" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="33" max="34" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="37" max="38" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="51" max="52" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="54" max="55" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="78" max="78" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="79" max="79" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="80" max="80" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="29" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="34" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="38" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="52" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:80" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -9251,7 +9447,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row customHeight="1" ht="17.25" r="3" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:80" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -9312,7 +9508,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:80" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -9374,7 +9570,7 @@
         <v>26</v>
       </c>
     </row>
-    <row ht="15.75" r="5" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:80" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -9431,7 +9627,7 @@
         <v>107</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:80" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -9483,7 +9679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:80" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -9522,7 +9718,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row ht="15.75" r="8" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:80" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -9573,7 +9769,7 @@
         <v>130</v>
       </c>
     </row>
-    <row ht="15.75" r="9" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:80" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -9662,25 +9858,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3:F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F9"/>
-    <hyperlink r:id="rId8" ref="E2"/>
-    <hyperlink r:id="rId9" ref="E3"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId10" ref="E4:E5"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId11" ref="E6:E9"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2" r:id="rId8"/>
+    <hyperlink ref="E3" r:id="rId9"/>
+    <hyperlink ref="E4:E5" r:id="rId10" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="E6:E9" r:id="rId11" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9689,51 +9885,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="31" max="32" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="32" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -11207,26 +11403,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11235,76 +11431,76 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="38.85546875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="42.5703125" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
-    <col min="45" max="46" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="48" max="48" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="32.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="38.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="42.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="41" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" x14ac:dyDescent="0.25">
@@ -11771,122 +11967,122 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="35.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="19" max="20" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="37.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
-    <col min="35" max="36" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="42" max="43" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="51" max="51" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="58" max="64" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="66" max="66" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="68" max="68" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="70" max="71" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="75" max="76" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="78" max="78" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="79" max="79" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="80" max="80" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="81" max="81" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="83" max="83" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="84" max="84" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="85" max="88" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="89" max="89" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="90" max="93" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="96" max="97" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="100" max="100" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="103" max="103" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="104" max="104" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="105" max="105" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="106" max="106" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="107" max="107" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="109" max="109" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="110" max="110" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="111" max="111" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="112" max="112" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="113" max="113" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="114" max="114" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="115" max="115" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="37.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="35.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="36" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="28.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="64" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="71" width="25" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="76" width="25" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="15" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="17" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="85" max="88" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="89" max="89" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="90" max="93" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="97" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="104" max="104" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="106" max="106" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="107" max="107" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="109" max="109" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="110" max="110" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="111" max="111" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="112" max="112" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="114" max="114" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="115" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:115" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:115" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -12233,7 +12429,7 @@
         <v>984</v>
       </c>
     </row>
-    <row ht="45" r="2" spans="1:115" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:115" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -12579,151 +12775,711 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.140625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="12.7109375" style="102" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="16" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="9.140625" style="102" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>1054</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>1035</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>1033</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>1034</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>1042</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>1036</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>1037</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>1038</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>1045</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>1039</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>1041</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="102" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K2" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="102" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="K3" s="102" t="s">
+        <v>1046</v>
+      </c>
+      <c r="L3" s="102" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M3" s="102" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N3" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="102" t="s">
+        <v>1048</v>
+      </c>
+      <c r="V3" s="102" t="s">
+        <v>1056</v>
+      </c>
+      <c r="W3" s="102" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="102" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="102" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K4" s="102" t="s">
+        <v>1046</v>
+      </c>
+      <c r="L4" s="102" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M4" s="102" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N4" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" s="102" t="s">
+        <v>1055</v>
+      </c>
+      <c r="V4" s="102" t="s">
+        <v>1061</v>
+      </c>
+      <c r="W4" s="102" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="102" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K5" s="102" t="s">
+        <v>1046</v>
+      </c>
+      <c r="L5" s="102" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M5" s="102" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N5" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="102" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="102" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K6" s="102" t="s">
+        <v>1046</v>
+      </c>
+      <c r="L6" s="102" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M6" s="102" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N6" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" s="102" t="s">
+        <v>1055</v>
+      </c>
+      <c r="V6" s="102" t="s">
+        <v>1061</v>
+      </c>
+      <c r="W6" s="102" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="102" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K7" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="102" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="102" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K8" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="102" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" s="102" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="102" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="J9" s="102">
+        <v>1431</v>
+      </c>
+      <c r="Z9" s="102" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="102" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="102" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="102" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K10" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="V14" s="25"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="112.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A1" s="103" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="103"/>
+      <c r="B2" s="103" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CH20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="95" zoomScaleNormal="95">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="42.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="30" max="31" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="34" max="35" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="48" max="49" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="51" max="52" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="78" max="78" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="79" max="80" bestFit="true" customWidth="true" width="40.140625" collapsed="true"/>
-    <col min="81" max="82" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="84" max="84" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="85" max="85" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="86" max="86" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="42.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="52" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="80" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="82" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -13024,7 +13780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="17.25" r="3" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:86" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -13071,7 +13827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -13112,7 +13868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row ht="15.75" r="5" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -13162,7 +13918,7 @@
         <v>107</v>
       </c>
     </row>
-    <row customHeight="1" ht="26.25" r="6" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:86" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -13208,7 +13964,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -13243,7 +13999,7 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
     </row>
-    <row ht="15.75" r="8" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -13290,7 +14046,7 @@
         <v>130</v>
       </c>
     </row>
-    <row ht="15.75" r="9" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -13435,7 +14191,7 @@
         <v>493</v>
       </c>
     </row>
-    <row ht="15.75" r="10" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>231</v>
       </c>
@@ -13482,7 +14238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="11" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>342</v>
       </c>
@@ -13529,7 +14285,7 @@
         <v>121</v>
       </c>
     </row>
-    <row ht="15.75" r="12" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>343</v>
       </c>
@@ -13582,7 +14338,7 @@
         <v>130</v>
       </c>
     </row>
-    <row ht="15.75" r="13" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>444</v>
       </c>
@@ -13689,7 +14445,7 @@
         <v>685</v>
       </c>
     </row>
-    <row ht="15.75" r="14" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>447</v>
       </c>
@@ -13733,7 +14489,7 @@
         <v>687</v>
       </c>
     </row>
-    <row ht="15.75" r="15" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>450</v>
       </c>
@@ -13775,7 +14531,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="16" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>452</v>
       </c>
@@ -13817,7 +14573,7 @@
       </c>
       <c r="BJ16" s="4"/>
     </row>
-    <row ht="15.75" r="17" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:81" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>743</v>
       </c>
@@ -13876,7 +14632,7 @@
         <v>750</v>
       </c>
     </row>
-    <row ht="15.75" r="18" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:81" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>752</v>
       </c>
@@ -13935,7 +14691,7 @@
         <v>759</v>
       </c>
     </row>
-    <row ht="15.75" r="19" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:81" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>760</v>
       </c>
@@ -13988,7 +14744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row ht="15.75" r="20" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:81" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>762</v>
       </c>
@@ -14034,82 +14790,82 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3:F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F9"/>
-    <hyperlink r:id="rId8" ref="E2"/>
-    <hyperlink r:id="rId9" ref="E3"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId10" ref="E4:E5"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId11" ref="E6:E9"/>
-    <hyperlink display="Newtglobal@123" r:id="rId12" ref="F10"/>
-    <hyperlink r:id="rId13" ref="E10"/>
-    <hyperlink display="Newtglobal@123" r:id="rId14" ref="F11"/>
-    <hyperlink r:id="rId15" ref="E11"/>
-    <hyperlink display="Newtglobal@123" r:id="rId16" ref="F12"/>
-    <hyperlink r:id="rId17" ref="E12"/>
-    <hyperlink display="Newtglobal@123" r:id="rId18" ref="F13"/>
-    <hyperlink r:id="rId19" ref="E13"/>
-    <hyperlink display="Newtglobal@123" r:id="rId20" ref="F14"/>
-    <hyperlink r:id="rId21" ref="E14"/>
-    <hyperlink display="Newtglobal@123" r:id="rId22" ref="F15"/>
-    <hyperlink r:id="rId23" ref="E15"/>
-    <hyperlink display="Newtglobal@123" r:id="rId24" ref="F16"/>
-    <hyperlink r:id="rId25" ref="E16"/>
-    <hyperlink display="Newtglobal@123" r:id="rId26" ref="F17"/>
-    <hyperlink r:id="rId27" ref="E17"/>
-    <hyperlink display="Newtglobal@123" r:id="rId28" ref="F18"/>
-    <hyperlink r:id="rId29" ref="E18"/>
-    <hyperlink display="Newtglobal@123" r:id="rId30" ref="F19"/>
-    <hyperlink r:id="rId31" ref="E19"/>
-    <hyperlink display="Newtglobal@123" r:id="rId32" ref="F20"/>
-    <hyperlink r:id="rId33" ref="E20"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2" r:id="rId8"/>
+    <hyperlink ref="E3" r:id="rId9"/>
+    <hyperlink ref="E4:E5" r:id="rId10" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="E6:E9" r:id="rId11" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F10" r:id="rId12" display="Newtglobal@123"/>
+    <hyperlink ref="E10" r:id="rId13"/>
+    <hyperlink ref="F11" r:id="rId14" display="Newtglobal@123"/>
+    <hyperlink ref="E11" r:id="rId15"/>
+    <hyperlink ref="F12" r:id="rId16" display="Newtglobal@123"/>
+    <hyperlink ref="E12" r:id="rId17"/>
+    <hyperlink ref="F13" r:id="rId18" display="Newtglobal@123"/>
+    <hyperlink ref="E13" r:id="rId19"/>
+    <hyperlink ref="F14" r:id="rId20" display="Newtglobal@123"/>
+    <hyperlink ref="E14" r:id="rId21"/>
+    <hyperlink ref="F15" r:id="rId22" display="Newtglobal@123"/>
+    <hyperlink ref="E15" r:id="rId23"/>
+    <hyperlink ref="F16" r:id="rId24" display="Newtglobal@123"/>
+    <hyperlink ref="E16" r:id="rId25"/>
+    <hyperlink ref="F17" r:id="rId26" display="Newtglobal@123"/>
+    <hyperlink ref="E17" r:id="rId27"/>
+    <hyperlink ref="F18" r:id="rId28" display="Newtglobal@123"/>
+    <hyperlink ref="E18" r:id="rId29"/>
+    <hyperlink ref="F19" r:id="rId30" display="Newtglobal@123"/>
+    <hyperlink ref="E19" r:id="rId31"/>
+    <hyperlink ref="F20" r:id="rId32" display="Newtglobal@123"/>
+    <hyperlink ref="E20" r:id="rId33"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="56.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="45.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="37.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="14" width="40.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="41.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="40.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="56.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="37.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="40.42578125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="41.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -14180,7 +14936,7 @@
         <v>183</v>
       </c>
     </row>
-    <row ht="15.75" r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -14319,7 +15075,7 @@
         <v>166</v>
       </c>
     </row>
-    <row ht="15.75" r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -14369,7 +15125,7 @@
         <v>194</v>
       </c>
     </row>
-    <row ht="15.75" r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -14419,7 +15175,7 @@
         <v>194</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -14469,7 +15225,7 @@
         <v>194</v>
       </c>
     </row>
-    <row ht="15.75" r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -14519,7 +15275,7 @@
         <v>641</v>
       </c>
     </row>
-    <row ht="15.75" r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -14616,27 +15372,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId8" ref="F9"/>
-    <hyperlink display="Newtglobal@123" r:id="rId9" ref="F10"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId10" ref="E2:E10"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="F9" r:id="rId8" display="Newtglobal@123"/>
+    <hyperlink ref="F10" r:id="rId9" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E10" r:id="rId10" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId11"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="P4"/>
+    <ignoredError sqref="P4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AB12"/>
   <sheetViews>
@@ -14646,36 +15402,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="46.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="32.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="29.7109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="33.28515625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="46" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="29.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="30" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="26" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="28.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -14803,7 +15559,7 @@
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row ht="15.75" r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -15338,28 +16094,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="E2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="E3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="E4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="E5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="E6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="E7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="E8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId8" ref="E9"/>
-    <hyperlink display="Newtglobal@123" r:id="rId9" ref="E11"/>
-    <hyperlink display="Newtglobal@123" r:id="rId10" ref="E10"/>
-    <hyperlink display="Newtglobal@123" r:id="rId11" ref="E12"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId12" ref="D2:D12"/>
+    <hyperlink ref="E2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="E3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="E4" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="E5" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="E6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="E7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="E8" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E9" r:id="rId8" display="Newtglobal@123"/>
+    <hyperlink ref="E11" r:id="rId9" display="Newtglobal@123"/>
+    <hyperlink ref="E10" r:id="rId10" display="Newtglobal@123"/>
+    <hyperlink ref="E12" r:id="rId11" display="Newtglobal@123"/>
+    <hyperlink ref="D2:D12" r:id="rId12" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="W9:X9 X6:X7 X10 X12"/>
+    <ignoredError sqref="W9:X9 X6:X7 X10 X12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AD9"/>
   <sheetViews>
@@ -15369,37 +16125,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="57.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="3.7109375" collapsed="true"/>
-    <col min="22" max="23" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="3.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="26" max="27" bestFit="true" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="27" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
@@ -15491,7 +16247,7 @@
         <v>183</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -15540,7 +16296,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row ht="30" r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -15589,7 +16345,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row ht="30" r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -15638,7 +16394,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row ht="30" r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -15716,7 +16472,7 @@
         <v>190</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -15796,7 +16552,7 @@
         <v>190</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -15868,7 +16624,7 @@
         <v>190</v>
       </c>
     </row>
-    <row ht="30" r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -15940,7 +16696,7 @@
         <v>190</v>
       </c>
     </row>
-    <row customHeight="1" ht="43.5" r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -15986,32 +16742,32 @@
       <c r="Y9" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="1" disablePrompts="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="Z2:Z6 AA2:AD9 Z9" type="list">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z6 AA2:AD9 Z9">
       <formula1>"ON,OFF"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F5:F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F2"/>
-    <hyperlink r:id="rId7" ref="D2"/>
-    <hyperlink display="https://10.133.43.10:8443/MessagingInstance/" r:id="rId8" ref="D3:D8"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId9" ref="E2:E8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId10" ref="F9"/>
-    <hyperlink r:id="rId11" ref="D9"/>
-    <hyperlink r:id="rId12" ref="E9"/>
+    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F5:F6" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="D2" r:id="rId7"/>
+    <hyperlink ref="D3:D8" r:id="rId8" display="https://10.133.43.10:8443/MessagingInstance/"/>
+    <hyperlink ref="E2:E8" r:id="rId9" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F9" r:id="rId10" display="Newtglobal@123"/>
+    <hyperlink ref="D9" r:id="rId11"/>
+    <hyperlink ref="E9" r:id="rId12"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId13"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Y8"/>
   <sheetViews>
@@ -16021,34 +16777,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -16145,7 +16901,7 @@
         <v>212</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -16181,7 +16937,7 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="5"/>
     </row>
-    <row ht="15.75" r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -16220,7 +16976,7 @@
       <c r="Q5" s="21"/>
       <c r="R5" s="5"/>
     </row>
-    <row ht="15.75" r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -16253,7 +17009,7 @@
       <c r="Q6" s="21"/>
       <c r="R6" s="5"/>
     </row>
-    <row ht="15.75" r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -16280,7 +17036,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row ht="15.75" r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -16318,27 +17074,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F7"/>
-    <hyperlink r:id="rId7" ref="E2"/>
-    <hyperlink r:id="rId8" ref="E3"/>
-    <hyperlink r:id="rId9" ref="E4"/>
-    <hyperlink r:id="rId10" ref="E5"/>
-    <hyperlink r:id="rId11" ref="E6"/>
-    <hyperlink r:id="rId12" ref="E7"/>
-    <hyperlink r:id="rId13" ref="E8"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="E2" r:id="rId7"/>
+    <hyperlink ref="E3" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId12"/>
+    <hyperlink ref="E8" r:id="rId13"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:Z9"/>
   <sheetViews>
@@ -16348,34 +17104,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="49.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -16530,7 +17286,7 @@
         <v>215</v>
       </c>
     </row>
-    <row ht="15.75" r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -16581,7 +17337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row ht="15.75" r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -16625,7 +17381,7 @@
       <c r="Q5" s="21"/>
       <c r="R5" s="5"/>
     </row>
-    <row ht="15.75" r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -16663,7 +17419,7 @@
       <c r="Q6" s="21"/>
       <c r="R6" s="5"/>
     </row>
-    <row ht="15.75" r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -16695,7 +17451,7 @@
         <v>218</v>
       </c>
     </row>
-    <row ht="15.75" r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -16746,7 +17502,7 @@
         <v>254</v>
       </c>
     </row>
-    <row ht="15.75" r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -16783,21 +17539,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F9"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId8" ref="E2:E9"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E9" r:id="rId8" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AJ16"/>
   <sheetViews>
@@ -16807,43 +17563,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="67.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="42.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="18" max="19" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="46.85546875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="67.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="42.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="46.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -17782,27 +18538,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="Newtglobal@123" r:id="rId1" ref="F2"/>
-    <hyperlink display="Newtglobal@123" r:id="rId2" ref="F3"/>
-    <hyperlink display="Newtglobal@123" r:id="rId3" ref="F4"/>
-    <hyperlink display="Newtglobal@123" r:id="rId4" ref="F5"/>
-    <hyperlink display="Newtglobal@123" r:id="rId5" ref="F6"/>
-    <hyperlink display="Newtglobal@123" r:id="rId6" ref="F7"/>
-    <hyperlink display="Newtglobal@123" r:id="rId7" ref="F8"/>
-    <hyperlink display="Newtglobal@123" r:id="rId8" ref="F9"/>
-    <hyperlink display="Newtglobal@123" r:id="rId9" ref="F10"/>
-    <hyperlink display="Newtglobal@123" r:id="rId10" ref="F11"/>
-    <hyperlink display="Newtglobal@123" r:id="rId11" ref="F12"/>
-    <hyperlink display="Newtglobal@123" r:id="rId12" ref="F13"/>
-    <hyperlink display="Newtglobal@123" r:id="rId13" ref="F14"/>
-    <hyperlink display="Newtglobal@123" r:id="rId14" ref="F15"/>
-    <hyperlink display="Newtglobal@123" r:id="rId15" ref="F16"/>
-    <hyperlink display="sonali.das@tatacommunications.com" r:id="rId16" ref="E2:E16"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123"/>
+    <hyperlink ref="F9" r:id="rId8" display="Newtglobal@123"/>
+    <hyperlink ref="F10" r:id="rId9" display="Newtglobal@123"/>
+    <hyperlink ref="F11" r:id="rId10" display="Newtglobal@123"/>
+    <hyperlink ref="F12" r:id="rId11" display="Newtglobal@123"/>
+    <hyperlink ref="F13" r:id="rId12" display="Newtglobal@123"/>
+    <hyperlink ref="F14" r:id="rId13" display="Newtglobal@123"/>
+    <hyperlink ref="F15" r:id="rId14" display="Newtglobal@123"/>
+    <hyperlink ref="F16" r:id="rId15" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E16" r:id="rId16" display="sonali.das@tatacommunications.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="AG7"/>
+    <ignoredError sqref="AG7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Customer - Price List Emailer scripts added
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="855" firstSheet="21" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="20" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Provisioning_Screen" sheetId="24" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3757" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3820" uniqueCount="1090">
   <si>
     <t>Username</t>
   </si>
@@ -3426,6 +3426,97 @@
   </si>
   <si>
     <t>RuleIDLinkValidation</t>
+  </si>
+  <si>
+    <t>Customer_Coverage_ServiceNameLst</t>
+  </si>
+  <si>
+    <t>Customer_Coverage_CustomerNameLst</t>
+  </si>
+  <si>
+    <t>Customer_Coverage_CustomerAccNameLst</t>
+  </si>
+  <si>
+    <t>21ST CENTURY TECHNOLOGIES LTD.</t>
+  </si>
+  <si>
+    <t>CENTURY_TEST_HTTP</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>[
+  {
+    "Region": "ASIA-PACIFIC",
+    "Country": "NEW ZEALAND",
+    "CountryCode": "",
+    "Operator": "2 DEGREES MOBILE LIMITED",
+    "Network": "TWO DEGREES MOBILE",
+    "MCCMNC": "53028, 53024",
+    "New Price": "0.0100",
+    "OldPrice": "",
+    "Change": "NEW COVERAGE",
+    "Effective Date": "15-09-2017",
+    "Features": "",
+    "Remarks": "",
+    "RouteType": ""
+  },
+  {
+    "Region": "INDIA",
+    "Country": "INDIA",
+    "CountryCode": "",
+    "Operator": "TELENOR (INDIA) COMMUNICATIONS PRIVATE LIMITED",
+    "Network": "UNITECH WIRELESS UTTAR PRADESH WEST",
+    "MCCMNC": "405844, 405818",
+    "New Price": "0.0001",
+    "OldPrice": "",
+    "Change": "",
+    "Effective Date": "14-09-2017",
+    "Features": "",
+    "Remarks": "",
+    "RouteType": ""
+  }
+]</t>
+  </si>
+  <si>
+    <t>Table_ResultData_Json</t>
+  </si>
+  <si>
+    <t>Customer&gt;Price List Emailer</t>
+  </si>
+  <si>
+    <t>Customer_Coverage_CustomerProductTxt</t>
+  </si>
+  <si>
+    <t>Customer_Coverage_TemplateLst</t>
+  </si>
+  <si>
+    <t>Mx-Test</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>Coloumn Name</t>
+  </si>
+  <si>
+    <t>Si.No</t>
+  </si>
+  <si>
+    <t>Customer_Coverage_Screen</t>
+  </si>
+  <si>
+    <t>EmailerTo</t>
+  </si>
+  <si>
+    <t>EmailerCC</t>
+  </si>
+  <si>
+    <t>Sonali.Das@tatacommunications.com</t>
+  </si>
+  <si>
+    <t>Maqdoom.Sharief@tatacommunications.com</t>
   </si>
 </sst>
 </file>
@@ -3871,7 +3962,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -4004,6 +4095,7 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
@@ -8616,9 +8708,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="137.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -11411,13 +11518,218 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>1070</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>1071</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>1072</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>1079</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>821</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>1086</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="102" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="102" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="O4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="102" t="s">
+        <v>1076</v>
+      </c>
+      <c r="Q4" s="102" t="s">
+        <v>1088</v>
+      </c>
+      <c r="R4" s="102" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -11426,7 +11738,7 @@
   <dimension ref="A1:BS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11979,7 +12291,7 @@
   <dimension ref="A1:DK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12834,8 +13146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13352,37 +13664,72 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="112.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" style="102"/>
+    <col min="2" max="2" width="26.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="112.140625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B1" s="106" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1" s="106" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="102">
+        <v>1</v>
+      </c>
+      <c r="B2" s="103" t="s">
         <v>1057</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="C2" s="103" t="s">
         <v>1058</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D2" s="102" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="103"/>
-      <c r="B2" s="103" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="102">
+        <v>2</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C3" s="103" t="s">
         <v>1059</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D3" s="102" t="s">
         <v>1060</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="102">
+        <v>3</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C4" s="102" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D4" s="102" t="s">
+        <v>1076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Price List emailer screen - Missing scripts added
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3820" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3834" uniqueCount="1092">
   <si>
     <t>Username</t>
   </si>
@@ -3517,6 +3517,26 @@
   </si>
   <si>
     <t>Maqdoom.Sharief@tatacommunications.com</t>
+  </si>
+  <si>
+    <t>Table_Haeders_Json</t>
+  </si>
+  <si>
+    <t>[
+  "Region",
+  "Country",  
+  "CountryCode",
+  "Operator",
+  "Network",
+  "MCCMNC",
+  "New Price",
+  "OldPrice",
+  "Change",
+  "Effective Date",
+  "Features",
+  "Remarks",
+  "RouteType"
+]</t>
   </si>
 </sst>
 </file>
@@ -3962,7 +3982,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -4096,6 +4116,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
@@ -11518,32 +11539,34 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="102" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="102" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.140625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.85546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37" style="102" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="38.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.28515625" style="102" customWidth="1"/>
+    <col min="17" max="17" width="255.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>36</v>
       </c>
@@ -11590,16 +11613,19 @@
         <v>821</v>
       </c>
       <c r="P1" s="23" t="s">
+        <v>1090</v>
+      </c>
+      <c r="Q1" s="23" t="s">
         <v>1077</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>1086</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>37</v>
       </c>
@@ -11618,23 +11644,21 @@
       <c r="G2" s="2" t="s">
         <v>1078</v>
       </c>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" t="s">
+      <c r="J2" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N2" s="107"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>38</v>
       </c>
@@ -11653,29 +11677,29 @@
       <c r="G3" s="2" t="s">
         <v>1078</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="102" t="s">
         <v>1073</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="102" t="s">
         <v>1074</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="102" t="s">
         <v>1075</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="102" t="s">
         <v>1081</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="102" t="s">
+      <c r="Q3" s="102" t="s">
         <v>1076</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>39</v>
       </c>
@@ -11694,32 +11718,73 @@
       <c r="G4" s="2" t="s">
         <v>1078</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="102" t="s">
         <v>1073</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="102" t="s">
         <v>1074</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="102" t="s">
         <v>1075</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="102" t="s">
         <v>1081</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="102" t="s">
+      <c r="Q4" s="102" t="s">
         <v>1076</v>
       </c>
-      <c r="Q4" s="102" t="s">
+      <c r="R4" s="102" t="s">
         <v>1088</v>
       </c>
-      <c r="R4" s="102" t="s">
+      <c r="S4" s="102" t="s">
         <v>1089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J5" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="102" t="s">
+        <v>1073</v>
+      </c>
+      <c r="L5" s="102" t="s">
+        <v>1074</v>
+      </c>
+      <c r="M5" s="102" t="s">
+        <v>1075</v>
+      </c>
+      <c r="N5" s="102" t="s">
+        <v>1081</v>
+      </c>
+      <c r="O5" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="102" t="s">
+        <v>1091</v>
       </c>
     </row>
   </sheetData>
@@ -11727,9 +11792,10 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Product Coverage Test Data Sheet Changes
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -3862,9 +3862,6 @@
     <t>MMX-Service</t>
   </si>
   <si>
-    <t>49101-COVERAGE-07-DEC-2017</t>
-  </si>
-  <si>
     <t>A-MOBILE</t>
   </si>
   <si>
@@ -3875,6 +3872,9 @@
   </si>
   <si>
     <t>37393-COVERAGE-26-OCT-2017</t>
+  </si>
+  <si>
+    <t>49206-COVERAGE-17-DEC-2017</t>
   </si>
 </sst>
 </file>
@@ -5595,8 +5595,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5917,17 +5917,17 @@
         <v>853</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>1197</v>
+        <v>1201</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="114" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
@@ -5984,7 +5984,7 @@
         <v>188</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>428</v>
@@ -6043,7 +6043,7 @@
         <v>154</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>239</v>
@@ -6052,7 +6052,7 @@
         <v>1177</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>1179</v>

</xml_diff>

<commit_message>
Product Price Test Data Sheet changes
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Provisioning_Screen" sheetId="24" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5744" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5899" uniqueCount="1222">
   <si>
     <t>Username</t>
   </si>
@@ -3876,6 +3876,66 @@
   <si>
     <t>49206-COVERAGE-17-DEC-2017</t>
   </si>
+  <si>
+    <t>Mcc_FilterLst</t>
+  </si>
+  <si>
+    <t>SuppliersFiltertxt</t>
+  </si>
+  <si>
+    <t>Ui Validation</t>
+  </si>
+  <si>
+    <t>Modifying Price,Adding new price for MT SMS</t>
+  </si>
+  <si>
+    <t>Modifying Price,Adding new price for MO SMS</t>
+  </si>
+  <si>
+    <t>Latest Price Card Validation</t>
+  </si>
+  <si>
+    <t>Validating Upload</t>
+  </si>
+  <si>
+    <t>UNITEL - The format for New Price is wrong - found in the row 1</t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>fdfdfd</t>
+  </si>
+  <si>
+    <t>49210-COVERAGE-17-DEC-2017</t>
+  </si>
+  <si>
+    <t>0.1232</t>
+  </si>
+  <si>
+    <t>01-10-2018</t>
+  </si>
+  <si>
+    <t>Mx-MO-2WLC</t>
+  </si>
+  <si>
+    <t>49104-SUBMITTED-07-DEC-2017</t>
+  </si>
+  <si>
+    <t>Mx-MT-2WLC</t>
+  </si>
+  <si>
+    <t>49095-COVERAGE-07-DEC-2017</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>14-06-2016</t>
+  </si>
+  <si>
+    <t>0.0064</t>
+  </si>
 </sst>
 </file>
 
@@ -3887,7 +3947,7 @@
     <numFmt numFmtId="166" formatCode="[$-14009]d\.m\.yy;@"/>
     <numFmt numFmtId="167" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4074,6 +4134,12 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="32">
@@ -4338,7 +4404,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -4490,6 +4556,9 @@
     <xf numFmtId="0" fontId="11" fillId="31" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
@@ -5595,7 +5664,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -8797,13 +8866,589 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>1202</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y1" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="AA1" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB1" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="AC1" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="AD1" s="38" t="s">
+        <v>308</v>
+      </c>
+      <c r="AE1" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="AF1" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="AG1" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="AH1" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+    </row>
+    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s">
+        <v>593</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="Q3" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="AA3" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB3" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="AC3" s="26">
+        <v>0.1148</v>
+      </c>
+      <c r="AD3" s="115">
+        <v>43370</v>
+      </c>
+      <c r="AE3" s="29" t="s">
+        <v>1213</v>
+      </c>
+      <c r="AF3" s="30" t="s">
+        <v>594</v>
+      </c>
+      <c r="AG3" s="30" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" t="s">
+        <v>593</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA4" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB4" s="115">
+        <v>43007</v>
+      </c>
+      <c r="AC4" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="AD4" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="AE4" s="30" t="s">
+        <v>590</v>
+      </c>
+      <c r="AF4" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="AG4" s="30" t="s">
+        <v>1214</v>
+      </c>
+      <c r="AH4" s="39"/>
+    </row>
+    <row r="5" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+    </row>
+    <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>457</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>458</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>1217</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>1218</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="N6" s="26"/>
+      <c r="O6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA6" s="30" t="s">
+        <v>1219</v>
+      </c>
+      <c r="AB6" s="31" t="s">
+        <v>1220</v>
+      </c>
+      <c r="AC6" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="AD6" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="AE6" s="29" t="s">
+        <v>1221</v>
+      </c>
+      <c r="AF6" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="AG6" s="30" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>456</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>1217</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>1218</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="29" t="s">
+        <v>1221</v>
+      </c>
+      <c r="AF7" s="117">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AG7" s="30"/>
+      <c r="AH7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1209</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>1217</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>1218</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="R8">
+        <v>412</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1210</v>
+      </c>
+      <c r="U8" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="V8" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1211</v>
+      </c>
+      <c r="X8" s="116">
+        <v>43119</v>
+      </c>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="28"/>
+      <c r="AI8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
+    <hyperlink ref="F4" r:id="rId4" display="Newtglobal@123"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
+    <hyperlink ref="E2:E7" r:id="rId7" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="F8" r:id="rId9" display="Newtglobal@123"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <ignoredErrors>
+    <ignoredError sqref="AE3:AF4 AA6 AE6:AF6 AE7" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added TopNDestination and Delivery Report test cases
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Provisioning_Screen" sheetId="24" r:id="rId1"/>
@@ -40,17 +40,19 @@
     <sheet name="ContactManagement_Screen" sheetId="37" r:id="rId31"/>
     <sheet name="Main" sheetId="38" r:id="rId32"/>
     <sheet name="Delivery_Statistics_Screen" sheetId="17" r:id="rId33"/>
+    <sheet name="TopN_Destination_Screen" sheetId="40" r:id="rId34"/>
+    <sheet name="DeliveryReport_Screen" sheetId="41" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">Delivery_Statistics_Screen!$A$1:$AG$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">Main!$A$1:$H$79</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6053" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6117" uniqueCount="1235">
   <si>
     <t>Username</t>
   </si>
@@ -3930,11 +3932,56 @@
   <si>
     <t>Mx-MO-2WSC</t>
   </si>
+  <si>
+    <t>Granularity</t>
+  </si>
+  <si>
+    <t>Granularity_Period</t>
+  </si>
+  <si>
+    <t>From_Date</t>
+  </si>
+  <si>
+    <t>Selection_Based_On</t>
+  </si>
+  <si>
+    <t>To_Date</t>
+  </si>
+  <si>
+    <t>Reporting&gt;TopN Destination</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>GOLD STONE SOURCING &amp; PROCUREMENT CONSULTANT</t>
+  </si>
+  <si>
+    <t>EMIRATES TELECOMMUNICATIONS GROUP COMPANY (ETISALAT GROUP) P.J.S.C.</t>
+  </si>
+  <si>
+    <t>Current Week-To-Date</t>
+  </si>
+  <si>
+    <t>MxMenapromo</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Reporting&gt;Delivery Report</t>
+  </si>
+  <si>
+    <t>Input Information is send to Message Box</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
@@ -4413,7 +4460,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -4567,19 +4614,22 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Excel Built-in Hyperlink" xfId="4"/>
-    <cellStyle name="Excel Built-in Normal" xfId="2"/>
-    <cellStyle name="Excel Built-in Normal 1" xfId="6"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="5"/>
-    <cellStyle name="Heading" xfId="7"/>
-    <cellStyle name="Heading1" xfId="8"/>
+    <cellStyle name="Excel Built-in Hyperlink" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel Built-in Normal 1" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Excel Built-in Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Heading" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Heading1" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Result" xfId="9"/>
-    <cellStyle name="Result2" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Result" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Result2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4637,7 +4687,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4670,9 +4720,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4705,6 +4772,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4880,7 +4964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BL10"/>
   <sheetViews>
@@ -5645,22 +5729,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="BA5" r:id="rId7"/>
-    <hyperlink ref="E2" r:id="rId8"/>
-    <hyperlink ref="E3" r:id="rId9"/>
-    <hyperlink ref="E4" r:id="rId10"/>
-    <hyperlink ref="E5" r:id="rId11"/>
-    <hyperlink ref="E6" r:id="rId12"/>
-    <hyperlink ref="E7" r:id="rId13"/>
-    <hyperlink ref="E8" r:id="rId14"/>
-    <hyperlink ref="E9" r:id="rId15"/>
-    <hyperlink ref="E10" r:id="rId16"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="BA5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E5" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E6" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E7" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -5668,7 +5752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AB7"/>
   <sheetViews>
@@ -6158,23 +6242,23 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:AB7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:AB7" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"ON,OFF"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="E2" r:id="rId7"/>
-    <hyperlink ref="E3" r:id="rId8"/>
-    <hyperlink ref="E4" r:id="rId9"/>
-    <hyperlink ref="E5" r:id="rId10"/>
-    <hyperlink ref="E6" r:id="rId11"/>
-    <hyperlink ref="E7" r:id="rId12"/>
+    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="F6" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="E2" r:id="rId7" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="E5" r:id="rId10" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
+    <hyperlink ref="E6" r:id="rId11" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0900-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -6182,7 +6266,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:P8"/>
   <sheetViews>
@@ -6575,21 +6659,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0A00-000006000000}"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0A00-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AE8"/>
   <sheetViews>
@@ -7165,14 +7249,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000004000000}"/>
+    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000005000000}"/>
+    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0B00-000006000000}"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0B00-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
@@ -7183,7 +7267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AG11"/>
   <sheetViews>
@@ -7795,14 +7879,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
+    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000004000000}"/>
+    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000005000000}"/>
+    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0C00-000006000000}"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0C00-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
@@ -7813,7 +7897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:AE8"/>
   <sheetViews>
@@ -8394,21 +8478,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com"/>
-    <hyperlink ref="D2" r:id="rId9"/>
-    <hyperlink ref="D3" r:id="rId10"/>
-    <hyperlink ref="D4" r:id="rId11"/>
-    <hyperlink ref="D5" r:id="rId12"/>
-    <hyperlink ref="D6" r:id="rId13"/>
-    <hyperlink ref="D7" r:id="rId14"/>
-    <hyperlink ref="D8" r:id="rId15"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="F5" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
+    <hyperlink ref="F7" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
+    <hyperlink ref="F8" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000004000000}"/>
+    <hyperlink ref="F6" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000005000000}"/>
+    <hyperlink ref="F4" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0D00-000006000000}"/>
+    <hyperlink ref="E2:E8" r:id="rId8" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0D00-000007000000}"/>
+    <hyperlink ref="D2" r:id="rId9" xr:uid="{00000000-0004-0000-0D00-000008000000}"/>
+    <hyperlink ref="D3" r:id="rId10" xr:uid="{00000000-0004-0000-0D00-000009000000}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{00000000-0004-0000-0D00-00000A000000}"/>
+    <hyperlink ref="D5" r:id="rId12" xr:uid="{00000000-0004-0000-0D00-00000B000000}"/>
+    <hyperlink ref="D6" r:id="rId13" xr:uid="{00000000-0004-0000-0D00-00000C000000}"/>
+    <hyperlink ref="D7" r:id="rId14" xr:uid="{00000000-0004-0000-0D00-00000D000000}"/>
+    <hyperlink ref="D8" r:id="rId15" xr:uid="{00000000-0004-0000-0D00-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -8419,7 +8503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8873,7 +8957,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -9442,15 +9526,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E7" r:id="rId7" display="sonali.das@tatacommunications.com"/>
-    <hyperlink ref="E8" r:id="rId8"/>
-    <hyperlink ref="F8" r:id="rId9" display="Newtglobal@123"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="F4" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000005000000}"/>
+    <hyperlink ref="E2:E7" r:id="rId7" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0F00-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0F00-000007000000}"/>
+    <hyperlink ref="F8" r:id="rId9" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0F00-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -9461,7 +9545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9473,7 +9557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9485,7 +9569,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11012,14 +11096,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CB9"/>
   <sheetViews>
@@ -11789,17 +11873,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2" r:id="rId8"/>
-    <hyperlink ref="E3" r:id="rId9"/>
-    <hyperlink ref="E4:E5" r:id="rId10" display="sonali.das@tatacommunications.com"/>
-    <hyperlink ref="E6:E9" r:id="rId11" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E3" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E4:E5" r:id="rId10" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E6:E9" r:id="rId11" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
@@ -11807,7 +11891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -12058,10 +12142,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-1300-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-1300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -12069,7 +12153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:BS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12614,15 +12698,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:DK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13422,7 +13506,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -13430,7 +13514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AX4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13915,19 +13999,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-1600-000002000000}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-1600-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-1600-000004000000}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{00000000-0004-0000-1600-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13939,7 +14023,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13951,7 +14035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13963,7 +14047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -14467,15 +14551,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-1A00-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-1A00-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-1A00-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-1A00-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-1A00-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-1A00-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-1A00-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-1A00-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -14483,7 +14567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14558,7 +14642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -14650,8 +14734,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-1C00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -14659,7 +14743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CH20"/>
   <sheetViews>
@@ -16047,39 +16131,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2" r:id="rId8"/>
-    <hyperlink ref="E3" r:id="rId9"/>
-    <hyperlink ref="E4:E5" r:id="rId10" display="sonali.das@tatacommunications.com"/>
-    <hyperlink ref="E6:E9" r:id="rId11" display="sonali.das@tatacommunications.com"/>
-    <hyperlink ref="F10" r:id="rId12" display="Newtglobal@123"/>
-    <hyperlink ref="E10" r:id="rId13"/>
-    <hyperlink ref="F11" r:id="rId14" display="Newtglobal@123"/>
-    <hyperlink ref="E11" r:id="rId15"/>
-    <hyperlink ref="F12" r:id="rId16" display="Newtglobal@123"/>
-    <hyperlink ref="E12" r:id="rId17"/>
-    <hyperlink ref="F13" r:id="rId18" display="Newtglobal@123"/>
-    <hyperlink ref="E13" r:id="rId19"/>
-    <hyperlink ref="F14" r:id="rId20" display="Newtglobal@123"/>
-    <hyperlink ref="E14" r:id="rId21"/>
-    <hyperlink ref="F15" r:id="rId22" display="Newtglobal@123"/>
-    <hyperlink ref="E15" r:id="rId23"/>
-    <hyperlink ref="F16" r:id="rId24" display="Newtglobal@123"/>
-    <hyperlink ref="E16" r:id="rId25"/>
-    <hyperlink ref="F17" r:id="rId26" display="Newtglobal@123"/>
-    <hyperlink ref="E17" r:id="rId27"/>
-    <hyperlink ref="F18" r:id="rId28" display="Newtglobal@123"/>
-    <hyperlink ref="E18" r:id="rId29"/>
-    <hyperlink ref="F19" r:id="rId30" display="Newtglobal@123"/>
-    <hyperlink ref="E19" r:id="rId31"/>
-    <hyperlink ref="F20" r:id="rId32" display="Newtglobal@123"/>
-    <hyperlink ref="E20" r:id="rId33"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="E3" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="E4:E5" r:id="rId10" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="E6:E9" r:id="rId11" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="F10" r:id="rId12" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="E10" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="F11" r:id="rId14" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="E11" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="F12" r:id="rId16" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="E12" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="F13" r:id="rId18" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="E13" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="F14" r:id="rId20" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="E14" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="F15" r:id="rId22" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="E15" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="F16" r:id="rId24" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="E16" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="F17" r:id="rId26" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="E17" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="F18" r:id="rId28" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="E18" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="F19" r:id="rId30" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="E19" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="F20" r:id="rId32" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="E20" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId34"/>
@@ -16087,7 +16171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -16193,8 +16277,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-1D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -16202,7 +16286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -16314,8 +16398,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-1E00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -16323,7 +16407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H79"/>
   <sheetViews>
@@ -18552,7 +18636,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H79">
+  <autoFilter ref="A1:H79" xr:uid="{00000000-0009-0000-0000-00001F000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Y"/>
@@ -18564,7 +18648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AG81"/>
   <sheetViews>
@@ -24311,14 +24395,292 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG81"/>
+  <autoFilter ref="A1:AG81" xr:uid="{00000000-0009-0000-0000-000020000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8823B205-5A65-4D62-BD2E-B78FFC2E0C5E}">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="101" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="101" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="101" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="101" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="101" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="101" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" style="101" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="101" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" style="101" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="101" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="101" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="101" customWidth="1"/>
+    <col min="14" max="15" width="20.5703125" style="101" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" style="101" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="101" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="101"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>1220</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>1222</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>1223</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>776</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H2" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="101">
+        <v>10</v>
+      </c>
+      <c r="L2" s="101" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="101" t="s">
+        <v>1226</v>
+      </c>
+      <c r="P2" s="101" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H3" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="101" t="s">
+        <v>1228</v>
+      </c>
+      <c r="J3" s="101" t="s">
+        <v>1229</v>
+      </c>
+      <c r="K3" s="101">
+        <v>10</v>
+      </c>
+      <c r="L3" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="M3" s="101" t="s">
+        <v>467</v>
+      </c>
+      <c r="N3" s="101" t="s">
+        <v>1230</v>
+      </c>
+      <c r="P3" s="101" t="s">
+        <v>1227</v>
+      </c>
+      <c r="Q3" s="101" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{31215716-9245-4AE0-93CC-B89BC798C007}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{CE12FBD0-50B1-45B2-B874-0E7073E75BF2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ABF64B-27D8-4242-8399-D9763276EB02}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H2" s="119" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H3" s="119" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{6871E697-C7B5-464E-B1F6-1FDF0A3AF98D}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{96855EC1-CE1A-4291-A9BF-8D37916022EA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:W10"/>
   <sheetViews>
@@ -24860,16 +25222,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="F9" r:id="rId8" display="Newtglobal@123"/>
-    <hyperlink ref="F10" r:id="rId9" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E10" r:id="rId10" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="E2:E10" r:id="rId10" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
@@ -24880,7 +25242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AB12"/>
   <sheetViews>
@@ -25601,18 +25963,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="E3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="E4" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="E5" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="E6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="E7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="E8" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E9" r:id="rId8" display="Newtglobal@123"/>
-    <hyperlink ref="E11" r:id="rId9" display="Newtglobal@123"/>
-    <hyperlink ref="E10" r:id="rId10" display="Newtglobal@123"/>
-    <hyperlink ref="E12" r:id="rId11" display="Newtglobal@123"/>
-    <hyperlink ref="D2:D12" r:id="rId12" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="E11" r:id="rId9" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="E10" r:id="rId10" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="D2:D12" r:id="rId12" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
@@ -25623,7 +25985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AD9"/>
   <sheetViews>
@@ -26251,23 +26613,23 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z6 AA2:AD9 Z9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z6 AA2:AD9 Z9" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"ON,OFF"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F5:F6" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="D2" r:id="rId7"/>
-    <hyperlink ref="D3:D8" r:id="rId8" display="https://10.133.43.10:8443/MessagingInstance/"/>
-    <hyperlink ref="E2:E8" r:id="rId9" display="sonali.das@tatacommunications.com"/>
-    <hyperlink ref="F9" r:id="rId10" display="Newtglobal@123"/>
-    <hyperlink ref="D9" r:id="rId11"/>
-    <hyperlink ref="E9" r:id="rId12"/>
+    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F5:F6" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="D2" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="D3:D8" r:id="rId8" display="https://10.133.43.10:8443/MessagingInstance/" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="E2:E8" r:id="rId9" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
@@ -26275,7 +26637,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Y8"/>
   <sheetViews>
@@ -26582,19 +26944,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="E2" r:id="rId7"/>
-    <hyperlink ref="E3" r:id="rId8"/>
-    <hyperlink ref="E4" r:id="rId9"/>
-    <hyperlink ref="E5" r:id="rId10"/>
-    <hyperlink ref="E6" r:id="rId11"/>
-    <hyperlink ref="E7" r:id="rId12"/>
-    <hyperlink ref="E8" r:id="rId13"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="E2" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="E5" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="E6" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="E8" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -26602,7 +26964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:Y9"/>
   <sheetViews>
@@ -27047,14 +27409,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E9" r:id="rId8" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="F9" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="E2:E9" r:id="rId8" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
@@ -27062,11 +27424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
@@ -28052,22 +28414,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123"/>
-    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123"/>
-    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123"/>
-    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123"/>
-    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123"/>
-    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123"/>
-    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123"/>
-    <hyperlink ref="F9" r:id="rId8" display="Newtglobal@123"/>
-    <hyperlink ref="F10" r:id="rId9" display="Newtglobal@123"/>
-    <hyperlink ref="F11" r:id="rId10" display="Newtglobal@123"/>
-    <hyperlink ref="F12" r:id="rId11" display="Newtglobal@123"/>
-    <hyperlink ref="F13" r:id="rId12" display="Newtglobal@123"/>
-    <hyperlink ref="F14" r:id="rId13" display="Newtglobal@123"/>
-    <hyperlink ref="F15" r:id="rId14" display="Newtglobal@123"/>
-    <hyperlink ref="F16" r:id="rId15" display="Newtglobal@123"/>
-    <hyperlink ref="E2:E16" r:id="rId16" display="sonali.das@tatacommunications.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0800-00000E000000}"/>
+    <hyperlink ref="E2:E16" r:id="rId16" display="sonali.das@tatacommunications.com" xr:uid="{00000000-0004-0000-0800-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>

</xml_diff>

<commit_message>
Adding MMX3.0 ( Delivery Statistics 3.0 ) automation scripts
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="29" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="30" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Provisioning_Screen" sheetId="24" r:id="rId1"/>
@@ -42,9 +42,11 @@
     <sheet name="Delivery_Statistics_Screen" sheetId="17" r:id="rId33"/>
     <sheet name="TopN_Destination_Screen" sheetId="40" r:id="rId34"/>
     <sheet name="DeliveryReport_Screen" sheetId="41" r:id="rId35"/>
+    <sheet name="Delivery_Statistics_Screen3.x" sheetId="42" r:id="rId36"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">Delivery_Statistics_Screen!$A$1:$AG$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="35" hidden="1">Delivery_Statistics_Screen3.x!$A$1:$AH$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">Main!$A$1:$H$79</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6117" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6231" uniqueCount="1262">
   <si>
     <t>Username</t>
   </si>
@@ -3976,6 +3978,87 @@
   </si>
   <si>
     <t>Input Information is send to Message Box</t>
+  </si>
+  <si>
+    <t>PeriodDate</t>
+  </si>
+  <si>
+    <t>SecondDrilldownHeaders_AckLatency</t>
+  </si>
+  <si>
+    <t>SecondDrilldownHeaders_E2ELatency</t>
+  </si>
+  <si>
+    <t>SecondDrilldownHeaders_PlatformLatency</t>
+  </si>
+  <si>
+    <t>SecondDrilldownHeaders_DeliveryLatency</t>
+  </si>
+  <si>
+    <t>https://mtmdevmblws01:8443/DeliveryStatisticsReportsWeb/</t>
+  </si>
+  <si>
+    <t>Reporting&gt;Delivery Statistics 3.0</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>LINKEDIN IRELAND</t>
+  </si>
+  <si>
+    <t>VIDEOCON TELECOMMUNICATIONS LIMITED</t>
+  </si>
+  <si>
+    <t>TST-MO</t>
+  </si>
+  <si>
+    <t>MTTSMSHUB3</t>
+  </si>
+  <si>
+    <t>Last 24 hours</t>
+  </si>
+  <si>
+    <t>Total Delivered~0-100 ms~0-100 ms %~100-200 ms~100-200 ms %~200-300 ms~200-300 ms %~300-400 ms~300-400 ms %~400-500 ms~400-500 ms %~500 ms - 1 sec~500 ms - 1 sec %~1 sec - 3 sec~1 sec - 3 sec %~&gt; 3 sec~&gt; 3 sec %</t>
+  </si>
+  <si>
+    <t>Total Delivered~0-5 Secs~0-5 Secs %~5-10 Secs~5-10 Secs %~10-15 Secs~10-15 Secs %~15-30 Secs~15-30 Secs %~30-60 Secs~30-60 Secs %~60-120 Secs~60-120 Secs %~120-180 Secs~120-180 Secs %~3-10 Min~3-10 Min %~&gt;10 Min~&gt;10 Min %</t>
+  </si>
+  <si>
+    <t>Total Delivered #~0-250 Msecs~0-250 Msecs %~250-500 Msecs~250-500 Msecs %~500 Msecs-1 Secs~500 Msecs-1 Secs %~1-3 Secs~1-3 Secs %~3-5 Secs~3-5 Secs %~5-10 Secs~5-10 Secs %~&gt; 10 Secs~&gt; 10 Secs %</t>
+  </si>
+  <si>
+    <t>Total Delivered~0-5 Secs~0-5 Secs %~5-10 Secs~5-10 Secs %~10-15 Secs~10-15 Secs %~15-30 Secs~15-30 Secs %~30-60 Secs~30-60 Secs %~60-120 Secs~60-120 Secs %~120-180 Secs~120-180 Secs %~3-10 Min~3-10 Min %~10-30 Min~10-30 Min %~30-360 Min~30-360 Min %~6-24 Hours~6-24 Hours %~&gt; 24 Hours~&gt; 24 Hours %</t>
+  </si>
+  <si>
+    <t>INFOBIP LIMITED</t>
+  </si>
+  <si>
+    <t>VODAFONE UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>Last 31 days</t>
+  </si>
+  <si>
+    <t>Customer~Customer Account~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Country~Destination~MCC~MNC~Supplier~Supplier Account~Attempted Success~Attempted Failure~Submitted~Submitted Success %~Submit Failure~Submitted Failure %~Enroute~Delivered Success~Delivered Success %~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Failure Reason~Failed~Failed %</t>
+  </si>
+  <si>
+    <t>Supplier~Supplier Account~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Country~Destination~MCC~MNC~Customer~Customer Account~Attempted Success~Attempted Failure~Submitted~Submitted Success %~Submit Failure~Submitted Failure %~Enroute~Delivered Success~Delivered Success %~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>TWILIO SWEDEN AB</t>
+  </si>
+  <si>
+    <t>Last 7 days</t>
   </si>
 </sst>
 </file>
@@ -24582,8 +24665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14ABF64B-27D8-4242-8399-D9763276EB02}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24676,6 +24759,421 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{96855EC1-CE1A-4291-A9BF-8D37916022EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5DC9AB-071B-4061-BA21-471EBE602838}">
+  <dimension ref="A1:AL11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="134.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="30.140625" customWidth="1"/>
+    <col min="33" max="33" width="38.42578125" customWidth="1"/>
+    <col min="34" max="34" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.85546875" customWidth="1"/>
+    <col min="36" max="36" width="36.5703125" customWidth="1"/>
+    <col min="37" max="37" width="43.28515625" customWidth="1"/>
+    <col min="38" max="38" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1089</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="L2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M2" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="R2" t="s">
+        <v>957</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>626</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>1249</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>622</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>623</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="M4" t="s">
+        <v>315</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1152</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>1249</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>1250</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>318</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1154</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1253</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>164</v>
+      </c>
+      <c r="O10" t="s">
+        <v>1260</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U11" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A40ABEB1-81DD-41EC-A0C1-0B9BD6029653}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{5C1A514D-146B-427A-97A8-91783F58BA32}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{8091AC44-C9DC-464E-9958-1223C8925B36}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Delivery statistics 3.0 uploaded
</commit_message>
<xml_diff>
--- a/data/Test_Data.xlsx
+++ b/data/Test_Data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4498421-3AFA-46DE-BAB5-F574C068AF6D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="30" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="868" firstSheet="32" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Provisioning_Screen" sheetId="24" r:id="rId1"/>
@@ -43,18 +44,19 @@
     <sheet name="TopN_Destination_Screen" sheetId="40" r:id="rId34"/>
     <sheet name="DeliveryReport_Screen" sheetId="41" r:id="rId35"/>
     <sheet name="Delivery_Statistics_Screen3.x" sheetId="42" r:id="rId36"/>
+    <sheet name="Supplier_Coverage_Screen3.x" sheetId="43" r:id="rId37"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="32" hidden="1">Delivery_Statistics_Screen!$A$1:$AG$81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="35" hidden="1">Delivery_Statistics_Screen3.x!$A$1:$AH$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="35" hidden="1">Delivery_Statistics_Screen3.x!$A$1:$AH$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">Main!$A$1:$H$79</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6231" uniqueCount="1262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6406" uniqueCount="1284">
   <si>
     <t>Username</t>
   </si>
@@ -4004,61 +4006,127 @@
     <t>MO</t>
   </si>
   <si>
-    <t>LINKEDIN IRELAND</t>
-  </si>
-  <si>
-    <t>VIDEOCON TELECOMMUNICATIONS LIMITED</t>
-  </si>
-  <si>
-    <t>TST-MO</t>
-  </si>
-  <si>
-    <t>MTTSMSHUB3</t>
-  </si>
-  <si>
-    <t>Last 24 hours</t>
+    <t>Total Delivered~0-5 Secs~0-5 Secs %~5-10 Secs~5-10 Secs %~10-15 Secs~10-15 Secs %~15-30 Secs~15-30 Secs %~30-60 Secs~30-60 Secs %~60-120 Secs~60-120 Secs %~120-180 Secs~120-180 Secs %~3-10 Min~3-10 Min %~&gt;10 Min~&gt;10 Min %</t>
+  </si>
+  <si>
+    <t>VODAFONE UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>Last 31 days</t>
+  </si>
+  <si>
+    <t>Customer~Customer Account~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Country~Destination~MCC~MNC~Supplier~Supplier Account~Attempted Success~Attempted Failure~Submitted~Submitted Success %~Submit Failure~Submitted Failure %~Enroute~Delivered Success~Delivered Success %~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Failure Reason~Failed~Failed %</t>
+  </si>
+  <si>
+    <t>Supplier~Supplier Account~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Country~Destination~MCC~MNC~Customer~Customer Account~Attempted Success~Attempted Failure~Submitted~Submitted Success %~Submit Failure~Submitted Failure %~Enroute~Delivered Success~Delivered Success %~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>TWILIO SWEDEN AB</t>
+  </si>
+  <si>
+    <t>Data_001</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>-- All Supplier Accounts --</t>
+  </si>
+  <si>
+    <t>-- All Suppliers --</t>
+  </si>
+  <si>
+    <t>-- All Coverage History --</t>
+  </si>
+  <si>
+    <t>MLNS</t>
+  </si>
+  <si>
+    <t>Total Delivered~0-100 ms~0-100 ms %~100-200 ms~100-200 ms %~200-300 ms~200-300 ms %~300-400 ms~300-400 ms %~400-500 ms~400-500 ms %~500 ms-1 sec~500 ms-1 sec %~1 sec-3 sec~1 sec-3 sec %~&gt;3 sec~&gt;3 sec %</t>
+  </si>
+  <si>
+    <t>Total Delivered~0-250 Msecs~0-250 Msecs %~250-500 Msecs~250-500 Msecs %~500 Msecs-1 Secs~500 Msecs-1 Secs %~1-3 Secs~1-3 Secs %~3-5 Secs~3-5 Secs %~5-10 Secs~5-10 Secs %~&gt;10 Secs~&gt;10 Secs %</t>
+  </si>
+  <si>
+    <t>Total Delivered~0-5 Secs~0-5 Secs %~5-10 Secs~5-10 Secs %~10-15 Secs~10-15 Secs %~15-30 Secs~15-30 Secs %~30-60 Secs~30-60 Secs %~60-120 Secs~60-120 Secs %~120-180 Secs~120-180 Secs %~3-10 Min~3-10 Min %~10-30 Min~10-30 Min %~30-360 Min~30-360 Min %~6-24 Hours~6-24 Hours %~&gt;24 Hours~&gt;24 Hours %</t>
+  </si>
+  <si>
+    <t>DRHandset</t>
+  </si>
+  <si>
+    <t>DR_SMSC</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>ConcatenationSupport</t>
+  </si>
+  <si>
+    <t>MNPSupport</t>
+  </si>
+  <si>
+    <t>DataCodingSupport</t>
+  </si>
+  <si>
+    <t>PreRegAN</t>
+  </si>
+  <si>
+    <t>FormatTemplateRegistration</t>
+  </si>
+  <si>
+    <t>TATforPreReg</t>
+  </si>
+  <si>
+    <t>ContentWhitelist</t>
+  </si>
+  <si>
+    <t>FormatTemplateContent</t>
+  </si>
+  <si>
+    <t>TATforContent</t>
+  </si>
+  <si>
+    <t>NoObjectionCertificate</t>
+  </si>
+  <si>
+    <t>TradeLicenseRequired</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>MOBISHASTRA TECHNOLOGIES LLC</t>
+  </si>
+  <si>
+    <t>2DEGREES_SMPP</t>
+  </si>
+  <si>
+    <t>Supplier&gt;Coverage Management 3.0</t>
   </si>
   <si>
     <t>Total Delivered~0-100 ms~0-100 ms %~100-200 ms~100-200 ms %~200-300 ms~200-300 ms %~300-400 ms~300-400 ms %~400-500 ms~400-500 ms %~500 ms - 1 sec~500 ms - 1 sec %~1 sec - 3 sec~1 sec - 3 sec %~&gt; 3 sec~&gt; 3 sec %</t>
   </si>
   <si>
-    <t>Total Delivered~0-5 Secs~0-5 Secs %~5-10 Secs~5-10 Secs %~10-15 Secs~10-15 Secs %~15-30 Secs~15-30 Secs %~30-60 Secs~30-60 Secs %~60-120 Secs~60-120 Secs %~120-180 Secs~120-180 Secs %~3-10 Min~3-10 Min %~&gt;10 Min~&gt;10 Min %</t>
-  </si>
-  <si>
-    <t>Total Delivered #~0-250 Msecs~0-250 Msecs %~250-500 Msecs~250-500 Msecs %~500 Msecs-1 Secs~500 Msecs-1 Secs %~1-3 Secs~1-3 Secs %~3-5 Secs~3-5 Secs %~5-10 Secs~5-10 Secs %~&gt; 10 Secs~&gt; 10 Secs %</t>
-  </si>
-  <si>
-    <t>Total Delivered~0-5 Secs~0-5 Secs %~5-10 Secs~5-10 Secs %~10-15 Secs~10-15 Secs %~15-30 Secs~15-30 Secs %~30-60 Secs~30-60 Secs %~60-120 Secs~60-120 Secs %~120-180 Secs~120-180 Secs %~3-10 Min~3-10 Min %~10-30 Min~10-30 Min %~30-360 Min~30-360 Min %~6-24 Hours~6-24 Hours %~&gt; 24 Hours~&gt; 24 Hours %</t>
-  </si>
-  <si>
-    <t>INFOBIP LIMITED</t>
-  </si>
-  <si>
-    <t>VODAFONE UNITED KINGDOM</t>
-  </si>
-  <si>
-    <t>Last 31 days</t>
-  </si>
-  <si>
-    <t>Customer~Customer Account~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
-  </si>
-  <si>
-    <t>Country~Destination~MCC~MNC~Supplier~Supplier Account~Attempted Success~Attempted Failure~Submitted~Submitted Success %~Submit Failure~Submitted Failure %~Enroute~Delivered Success~Delivered Success %~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
-  </si>
-  <si>
-    <t>Failure Reason~Failed~Failed %</t>
-  </si>
-  <si>
-    <t>Supplier~Supplier Account~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
-  </si>
-  <si>
-    <t>Country~Destination~MCC~MNC~Customer~Customer Account~Attempted Success~Attempted Failure~Submitted~Submitted Success %~Submit Failure~Submitted Failure %~Enroute~Delivered Success~Delivered Success %~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
-  </si>
-  <si>
-    <t>TWILIO SWEDEN AB</t>
-  </si>
-  <si>
-    <t>Last 7 days</t>
+    <t>Country~Destination~Attempted Success~Attempted Failure~Submitted Success~Submitted Failure~Submitted %~Enroute~Delivered Success~Delivered Failure~Delivered %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
+  </si>
+  <si>
+    <t>Customer~Customer Account~MCC~MNC~Attempted Success~Attempted Failure~Submitted~Submit Failure~Submitted Failure %~Enroute~Delivered Succes~Delivered Failure~Delivered Failure %~E2E Latency (s)~Ack Latency (ms)~Platform Latency (ms)~Delivery Latency (s)</t>
   </si>
 </sst>
 </file>
@@ -4071,7 +4139,7 @@
     <numFmt numFmtId="166" formatCode="[$-14009]d\.m\.yy;@"/>
     <numFmt numFmtId="167" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4270,6 +4338,38 @@
       <color rgb="FF0000FF"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="32">
@@ -4543,7 +4643,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -4700,6 +4800,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Excel Built-in Hyperlink" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -18735,8 +18840,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AG81"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24764,17 +24869,17 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5DC9AB-071B-4061-BA21-471EBE602838}">
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="41.28515625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -24788,7 +24893,7 @@
     <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="20" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="23.140625" customWidth="1"/>
     <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -24928,7 +25033,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>94</v>
@@ -24954,70 +25059,52 @@
       <c r="I2" t="s">
         <v>1241</v>
       </c>
-      <c r="L2" t="s">
-        <v>317</v>
-      </c>
       <c r="M2" t="s">
         <v>318</v>
       </c>
-      <c r="N2" t="s">
-        <v>1242</v>
-      </c>
       <c r="O2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>467</v>
+      </c>
+      <c r="R2" t="s">
+        <v>468</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>1243</v>
       </c>
-      <c r="P2" t="s">
-        <v>1244</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1073</v>
-      </c>
-      <c r="R2" t="s">
-        <v>957</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1245</v>
-      </c>
-      <c r="T2" t="s">
-        <v>1246</v>
-      </c>
-      <c r="U2" t="s">
-        <v>1247</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>626</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>1064</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>1067</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>1065</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>1248</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>1249</v>
-      </c>
       <c r="AK2" t="s">
-        <v>1250</v>
+        <v>1259</v>
       </c>
       <c r="AL2" t="s">
-        <v>1251</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D3" t="s">
         <v>1240</v>
@@ -25037,49 +25124,55 @@
       <c r="I3" t="s">
         <v>1241</v>
       </c>
+      <c r="M3" t="s">
+        <v>315</v>
+      </c>
       <c r="O3" t="s">
-        <v>1252</v>
+        <v>1251</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1152</v>
       </c>
       <c r="Q3" t="s">
         <v>1154</v>
       </c>
       <c r="R3" t="s">
-        <v>1253</v>
+        <v>1244</v>
       </c>
       <c r="U3" t="s">
-        <v>1254</v>
+        <v>1245</v>
       </c>
       <c r="AE3" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="AF3" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="AH3" t="s">
-        <v>1257</v>
+        <v>1248</v>
       </c>
       <c r="AI3" t="s">
-        <v>1248</v>
+        <v>1281</v>
       </c>
       <c r="AJ3" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="AK3" t="s">
-        <v>1250</v>
+        <v>1259</v>
       </c>
       <c r="AL3" t="s">
-        <v>1251</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D4" t="s">
         <v>1240</v>
@@ -25100,80 +25193,862 @@
         <v>1241</v>
       </c>
       <c r="M4" t="s">
-        <v>315</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1229</v>
+        <v>166</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1244</v>
       </c>
       <c r="U4" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="AE4" t="s">
-        <v>1258</v>
+        <v>1282</v>
       </c>
       <c r="AF4" t="s">
-        <v>1259</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>1257</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>1248</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>1249</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>1250</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="M9" t="s">
-        <v>318</v>
-      </c>
-      <c r="O9" t="s">
-        <v>1252</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>1154</v>
-      </c>
-      <c r="R9" t="s">
-        <v>1253</v>
-      </c>
-      <c r="U9" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="M10" t="s">
-        <v>164</v>
-      </c>
-      <c r="O10" t="s">
-        <v>1260</v>
-      </c>
-      <c r="U10" t="s">
-        <v>1261</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="U11" t="s">
-        <v>1247</v>
+        <v>1283</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{A40ABEB1-81DD-41EC-A0C1-0B9BD6029653}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{5C1A514D-146B-427A-97A8-91783F58BA32}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{8091AC44-C9DC-464E-9958-1223C8925B36}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{951D2F5A-E1D1-4957-8D80-C803CD7791DF}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{739996E1-7246-4743-8322-37C6B9FA1F14}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{1A666A4C-BF8D-4C90-BEF5-760F53516BA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267BCD3E-260D-4315-959A-6CD9DFA7D3DA}">
+  <dimension ref="A1:AQ9"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="3.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="41.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="123" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="123" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="123" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="123" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" s="123" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="123" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="123" t="s">
+        <v>167</v>
+      </c>
+      <c r="R1" s="123" t="s">
+        <v>168</v>
+      </c>
+      <c r="S1" s="123" t="s">
+        <v>169</v>
+      </c>
+      <c r="T1" s="123" t="s">
+        <v>684</v>
+      </c>
+      <c r="U1" s="124" t="s">
+        <v>170</v>
+      </c>
+      <c r="V1" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="W1" s="124" t="s">
+        <v>1277</v>
+      </c>
+      <c r="X1" s="124" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y1" s="124" t="s">
+        <v>1261</v>
+      </c>
+      <c r="Z1" s="124" t="s">
+        <v>1262</v>
+      </c>
+      <c r="AA1" s="124" t="s">
+        <v>1265</v>
+      </c>
+      <c r="AB1" s="124" t="s">
+        <v>1266</v>
+      </c>
+      <c r="AC1" s="124" t="s">
+        <v>1267</v>
+      </c>
+      <c r="AD1" s="121" t="s">
+        <v>1268</v>
+      </c>
+      <c r="AE1" s="121" t="s">
+        <v>1263</v>
+      </c>
+      <c r="AF1" s="121" t="s">
+        <v>1269</v>
+      </c>
+      <c r="AG1" s="121" t="s">
+        <v>1270</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>1271</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>1272</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>1273</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>1274</v>
+      </c>
+      <c r="AL1" s="17" t="s">
+        <v>1275</v>
+      </c>
+      <c r="AM1" s="122" t="s">
+        <v>1264</v>
+      </c>
+      <c r="AN1" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="AO1" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP1" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="AQ1" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>685</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="K2" s="120" t="s">
+        <v>1255</v>
+      </c>
+      <c r="L2" s="120" t="s">
+        <v>1254</v>
+      </c>
+      <c r="M2" s="120" t="s">
+        <v>1256</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+    </row>
+    <row r="3" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="K3" s="120" t="s">
+        <v>1255</v>
+      </c>
+      <c r="L3" s="120" t="s">
+        <v>1254</v>
+      </c>
+      <c r="M3" s="120" t="s">
+        <v>1256</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+    </row>
+    <row r="4" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="K4" s="120" t="s">
+        <v>1255</v>
+      </c>
+      <c r="L4" s="120" t="s">
+        <v>1254</v>
+      </c>
+      <c r="M4" s="120" t="s">
+        <v>1256</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+    </row>
+    <row r="5" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>688</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1276</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>543</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>184</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="T6" t="s">
+        <v>531</v>
+      </c>
+      <c r="U6" t="s">
+        <v>121</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="W6" t="s">
+        <v>183</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>184</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>690</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>184</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>690</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>184</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" t="s">
+        <v>821</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>823</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN9 AN5:AN6 AO5:AQ9 AN2:AQ4" xr:uid="{890065BC-97DB-4542-A3DA-E6EAC283E7C1}">
+      <formula1>"ON,OFF"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" display="Newtglobal@123" xr:uid="{31139429-02CD-4D1A-9F3F-02331206EA2B}"/>
+    <hyperlink ref="F5:F6" r:id="rId2" display="Newtglobal@123" xr:uid="{B5212FD0-957F-441B-91B0-6B297C602061}"/>
+    <hyperlink ref="F7" r:id="rId3" display="Newtglobal@123" xr:uid="{8662B842-E709-4594-A4C1-833F61740AD1}"/>
+    <hyperlink ref="F8" r:id="rId4" display="Newtglobal@123" xr:uid="{DE49527C-FF56-496D-9902-BC7B61D26FF3}"/>
+    <hyperlink ref="F3" r:id="rId5" display="Newtglobal@123" xr:uid="{532DB05E-F563-4E60-8397-F6238F07A1A7}"/>
+    <hyperlink ref="F2" r:id="rId6" display="Newtglobal@123" xr:uid="{19491B21-615F-49A9-8752-4B16DAC7F085}"/>
+    <hyperlink ref="D2" r:id="rId7" xr:uid="{82A0ADA2-DF54-4548-87C3-E651E1AC33F7}"/>
+    <hyperlink ref="D3:D8" r:id="rId8" display="https://10.133.43.10:8443/MessagingInstance/" xr:uid="{CE655653-A829-48B7-8CA9-D7E3535ED87A}"/>
+    <hyperlink ref="E2:E8" r:id="rId9" display="sonali.das@tatacommunications.com" xr:uid="{8FEBBBE4-88EE-475B-8F60-0075A00AC776}"/>
+    <hyperlink ref="F9" r:id="rId10" display="Newtglobal@123" xr:uid="{37B48C4D-812D-4A2C-A7A0-814D04F2BD9C}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{2014FCD1-8DC7-416B-AEDD-85FB7F3D9BEC}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{D8DA0916-53EE-4D8E-8691-D236140D0C55}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -26485,10 +27360,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27109,9 +27984,58 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
+    <row r="10" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>685</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="K10" s="120" t="s">
+        <v>1255</v>
+      </c>
+      <c r="L10" s="120" t="s">
+        <v>1254</v>
+      </c>
+      <c r="M10" s="120" t="s">
+        <v>1256</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z6 AA2:AD9 Z9" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z6 AA2:AD10 Z9:Z10" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"ON,OFF"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27128,9 +28052,12 @@
     <hyperlink ref="F9" r:id="rId10" display="Newtglobal@123" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
     <hyperlink ref="D9" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
     <hyperlink ref="E9" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="F10" r:id="rId13" display="Newtglobal@123" xr:uid="{99646ADE-1EA3-4BDB-BB60-0037A6E08790}"/>
+    <hyperlink ref="D10" r:id="rId14" xr:uid="{1CDD3195-C59E-407D-8ECD-C76E2A68A10C}"/>
+    <hyperlink ref="E10" r:id="rId15" xr:uid="{F149C6FF-F4AD-47B8-8268-10D9B39C2AAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>